<commit_message>
Dealing with the mysteriously inserted double-spaces in Excel
</commit_message>
<xml_diff>
--- a/myStudies/RothConversion.xlsx
+++ b/myStudies/RothConversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkrat\git\MyStudiesRepo\myStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0395468-06C6-445F-B1DB-C6B2A5F9A2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77E0498-FA7A-441C-A1B6-823DBDA78C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" activeTab="1" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statics" sheetId="38" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="121">
   <si>
     <t>Description</t>
   </si>
@@ -395,13 +395,25 @@
     <t>IRA Divisor First Year</t>
   </si>
   <si>
+    <t>Social Security  First Year</t>
+  </si>
+  <si>
+    <t>IRMAA Multipliers  First Year</t>
+  </si>
+  <si>
     <t>OPM</t>
   </si>
   <si>
     <t>TransAmerica Annuity</t>
   </si>
   <si>
+    <t>Long Term Rate First Year</t>
+  </si>
+  <si>
     <t>Medicare Part B Standard Premium First Year</t>
+  </si>
+  <si>
+    <t>Tax Brackets First  Year</t>
   </si>
   <si>
     <t>Final Year</t>
@@ -1991,8 +2003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8746EC-93A7-4CC1-BFC6-CA309B41AD35}">
   <dimension ref="A1:I258"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,7 +2048,7 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="70" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B3" s="71"/>
       <c r="C3" s="72"/>
@@ -2080,7 +2092,7 @@
     </row>
     <row r="7" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="79" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="72"/>
@@ -2386,7 +2398,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B35" s="95" t="s">
         <v>93</v>
@@ -2398,7 +2410,7 @@
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B36" s="95" t="s">
         <v>92</v>
@@ -2415,7 +2427,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B38" s="22">
         <f>12*2578.1</f>
@@ -2425,7 +2437,7 @@
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B39" s="22">
         <f>71065.98-50692.01</f>
@@ -2526,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFC4955-0F80-43F5-88A1-E586421548F7}">
   <dimension ref="A1:I252"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,9 +2560,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="str">
-        <f>TRIM("Tax Brackets First  Year")</f>
-        <v>Tax Brackets First Year</v>
+      <c r="A1" s="79" t="s">
+        <v>119</v>
       </c>
       <c r="B1" s="71"/>
       <c r="C1" s="72"/>
@@ -2617,9 +2628,8 @@
       <c r="C8" s="20"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="79" t="str">
-        <f>TRIM("Long Term Rate First Year")</f>
-        <v>Long Term Rate First Year</v>
+      <c r="A9" s="79" t="s">
+        <v>117</v>
       </c>
       <c r="B9" s="71"/>
       <c r="C9" s="72"/>
@@ -2650,9 +2660,8 @@
       <c r="C12" s="20"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="79" t="str">
-        <f>TRIM("Social Security  First Year")</f>
-        <v>Social Security First Year</v>
+      <c r="A13" s="79" t="s">
+        <v>113</v>
       </c>
       <c r="B13" s="71"/>
       <c r="C13" s="72"/>
@@ -2680,9 +2689,8 @@
       <c r="B16" s="22"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="79" t="str">
-        <f>TRIM("IRMAA Multipliers  First Year")</f>
-        <v>IRMAA Multipliers First Year</v>
+      <c r="A17" s="79" t="s">
+        <v>114</v>
       </c>
       <c r="B17" s="71"/>
       <c r="C17" s="72"/>

</xml_diff>

<commit_message>
Everything is read in.
</commit_message>
<xml_diff>
--- a/myStudies/RothConversion.xlsx
+++ b/myStudies/RothConversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkrat\git\MyStudiesRepo\myStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77E0498-FA7A-441C-A1B6-823DBDA78C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E62D12C-EF17-4311-ACDE-5FC2B664F8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" activeTab="1" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" activeTab="2" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statics" sheetId="38" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="126">
   <si>
     <t>Description</t>
   </si>
@@ -287,12 +287,6 @@
     <t>Today's Date</t>
   </si>
   <si>
-    <t>Fidelity Consolidated 2024 Year-to-Date Tax Activity</t>
-  </si>
-  <si>
-    <t>Fidelity Consolidated 2024 Ordinary Dividends and Distributions</t>
-  </si>
-  <si>
     <t>IRA Withdrawal Line is "Accent1"</t>
   </si>
   <si>
@@ -341,6 +335,9 @@
     <t>IRA Age of RMD</t>
   </si>
   <si>
+    <t>Tax Brackets</t>
+  </si>
+  <si>
     <t>Summaries of Java Input (With no Optional IRA Withdrawal)</t>
   </si>
   <si>
@@ -417,6 +414,24 @@
   </si>
   <si>
     <t>Final Year</t>
+  </si>
+  <si>
+    <t>Inflation</t>
+  </si>
+  <si>
+    <t>Investments</t>
+  </si>
+  <si>
+    <t>Growth Rate Year</t>
+  </si>
+  <si>
+    <t>Growth Rate</t>
+  </si>
+  <si>
+    <t>Fidelity Consolidated Year-to-Date Tax Activity</t>
+  </si>
+  <si>
+    <t>Fidelity Consolidated Ordinary Dividends and Distributions</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1425,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1635,6 +1650,11 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2003,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8746EC-93A7-4CC1-BFC6-CA309B41AD35}">
   <dimension ref="A1:I258"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2026,7 +2046,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="71"/>
       <c r="C1" s="72"/>
@@ -2048,7 +2068,7 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="70" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" s="71"/>
       <c r="C3" s="72"/>
@@ -2068,7 +2088,7 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" s="74"/>
       <c r="C5" s="75"/>
@@ -2092,7 +2112,7 @@
     </row>
     <row r="7" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="79" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="72"/>
@@ -2115,7 +2135,7 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="70" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="71"/>
       <c r="C9" s="72"/>
@@ -2127,7 +2147,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" s="94">
         <v>19661</v>
@@ -2138,7 +2158,7 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B11" s="94">
         <v>20859</v>
@@ -2150,7 +2170,7 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="70" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="71"/>
       <c r="C12" s="72"/>
@@ -2160,19 +2180,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" s="95" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="95" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="4" t="s">
@@ -2181,10 +2201,10 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" s="95" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="4" t="s">
@@ -2193,7 +2213,7 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="70" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B16" s="71"/>
       <c r="C16" s="72"/>
@@ -2201,7 +2221,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2">
         <v>73</v>
@@ -2213,7 +2233,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2">
         <v>73</v>
@@ -2222,7 +2242,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="70" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="71"/>
       <c r="C19" s="72"/>
@@ -2232,7 +2252,7 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="2">
         <v>2019</v>
@@ -2241,109 +2261,109 @@
     </row>
     <row r="21" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" s="71"/>
       <c r="C21" s="72"/>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="2">
         <v>21.2</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23" s="71"/>
       <c r="C23" s="72"/>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B24" s="22">
         <v>41925.5</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25" s="22">
         <v>2082478.98</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" s="22">
         <v>1049867.8400000001</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" s="71"/>
       <c r="C27" s="72"/>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B28" s="22">
         <v>41925</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B29" s="22">
         <v>2200000</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B30" s="22">
         <v>1009000</v>
@@ -2352,7 +2372,7 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" s="70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B31" s="71"/>
       <c r="C31" s="72"/>
@@ -2362,7 +2382,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B32" s="22">
         <f>10*1487.9</f>
@@ -2375,7 +2395,7 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B33" s="22">
         <f>12*2578.9</f>
@@ -2388,7 +2408,7 @@
     </row>
     <row r="34" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A34" s="70" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B34" s="71"/>
       <c r="C34" s="72"/>
@@ -2398,28 +2418,28 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B35" s="95" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="66" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B36" s="95" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A37" s="70" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" s="71"/>
       <c r="C37" s="72"/>
@@ -2427,7 +2447,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B38" s="22">
         <f>12*2578.1</f>
@@ -2437,7 +2457,7 @@
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B39" s="22">
         <f>71065.98-50692.01</f>
@@ -2447,14 +2467,14 @@
     </row>
     <row r="40" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B40" s="77"/>
       <c r="C40" s="78"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A41" s="34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B41" s="35">
         <v>-10950</v>
@@ -2463,7 +2483,7 @@
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B42" s="24">
         <v>-17755</v>
@@ -2471,20 +2491,67 @@
       <c r="C42" s="25"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="67" t="s">
-        <v>99</v>
-      </c>
-      <c r="B43" s="68"/>
-      <c r="C43" s="69"/>
-    </row>
-    <row r="56" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="79" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="71"/>
+      <c r="C43" s="72"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" s="96">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" s="96">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="96">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="79" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" s="71"/>
+      <c r="C47" s="72"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="97" t="str">
+        <f>A46</f>
+        <v>Tax Brackets</v>
+      </c>
+      <c r="B48" s="98">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="68"/>
+      <c r="C49" s="69"/>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I59" s="3"/>
     </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I60" s="5"/>
     </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I61" s="5"/>
     </row>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2511,7 +2578,7 @@
     <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A5:C5"/>
@@ -2522,12 +2589,14 @@
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A49:C49"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A43:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2536,10 +2605,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFC4955-0F80-43F5-88A1-E586421548F7}">
-  <dimension ref="A1:I252"/>
+  <dimension ref="A1:I258"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2561,7 +2630,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="71"/>
       <c r="C1" s="72"/>
@@ -2629,7 +2698,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="71"/>
       <c r="C9" s="72"/>
@@ -2661,7 +2730,7 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" s="71"/>
       <c r="C13" s="72"/>
@@ -2688,14 +2757,14 @@
       </c>
       <c r="B16" s="22"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="79" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17" s="71"/>
       <c r="C17" s="72"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <v>1</v>
       </c>
@@ -2703,7 +2772,7 @@
         <v>210000</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <v>1.4</v>
       </c>
@@ -2711,7 +2780,7 @@
         <v>264000</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>2</v>
       </c>
@@ -2719,7 +2788,7 @@
         <v>330000</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
         <v>2.6</v>
       </c>
@@ -2727,7 +2796,7 @@
         <v>394000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>3.2</v>
       </c>
@@ -2735,58 +2804,58 @@
         <v>750000</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21">
         <v>3.4</v>
       </c>
       <c r="B23" s="58"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="67" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B24" s="68"/>
       <c r="C24" s="69"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I31" s="5"/>
-    </row>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="5"/>
+    </row>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D189" s="1"/>
-    </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D194" s="1"/>
-    </row>
-    <row r="200" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D195" s="1"/>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D200" s="1"/>
+    </row>
+    <row r="206" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A24:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2798,8 +2867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD54838-E504-4CBA-8D4E-DD881A64EA8E}">
   <dimension ref="A1:I254"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:C47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2821,7 +2890,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="75"/>
@@ -3086,7 +3155,7 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="67" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="B27" s="68"/>
       <c r="C27" s="69"/>
@@ -3305,7 +3374,7 @@
     </row>
     <row r="47" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A47" s="67" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B47" s="68"/>
       <c r="C47" s="69"/>
@@ -3315,7 +3384,7 @@
     </row>
     <row r="49" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="67" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B49" s="68"/>
       <c r="C49" s="69"/>
@@ -4857,7 +4926,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="68"/>
       <c r="C1" s="69"/>
@@ -4874,7 +4943,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed the spreadsheet of course.
</commit_message>
<xml_diff>
--- a/myStudies/RothConversion.xlsx
+++ b/myStudies/RothConversion.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkrat\git\MyStudiesRepo\myStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9E34E9-27C6-4E2E-B406-CCDA0A0EFAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903200E9-1BC0-4FB6-8CED-14B319E34361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="16470" tabRatio="735" activeTab="2" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statics" sheetId="38" r:id="rId1"/>
     <sheet name="Brackets" sheetId="39" r:id="rId2"/>
-    <sheet name="Fidelity" sheetId="41" r:id="rId3"/>
+    <sheet name="Investments" sheetId="41" r:id="rId3"/>
     <sheet name="Outputsx" sheetId="40" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="OI_ROW" localSheetId="1">_xlfn.XMATCH(#REF!,Brackets!#REF!,-1,2)</definedName>
-    <definedName name="OI_ROW" localSheetId="2">_xlfn.XMATCH(#REF!,Fidelity!#REF!,-1,2)</definedName>
+    <definedName name="OI_ROW" localSheetId="2">_xlfn.XMATCH(#REF!,Investments!#REF!,-1,2)</definedName>
     <definedName name="OI_ROW" localSheetId="3">_xlfn.XMATCH(#REF!,Outputsx!#REF!,-1,2)</definedName>
     <definedName name="OI_ROW" localSheetId="0">_xlfn.XMATCH(#REF!,Statics!#REF!,-1,2)</definedName>
     <definedName name="OI_ROW">_xlfn.XMATCH(#REF!,#REF!,-1,2)</definedName>
@@ -350,12 +350,6 @@
     <t>Investments</t>
   </si>
   <si>
-    <t>Fidelity Consolidated Year-to-Date Tax Activity</t>
-  </si>
-  <si>
-    <t>Fidelity Consolidated Ordinary Dividends and Distributions</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -423,6 +417,12 @@
   </si>
   <si>
     <t>Part B Premium Current Year</t>
+  </si>
+  <si>
+    <t>Consolidated Year-to-Date Tax Activity</t>
+  </si>
+  <si>
+    <t>Consolidated Ordinary Dividends and Distributions</t>
   </si>
 </sst>
 </file>
@@ -2023,7 +2023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8746EC-93A7-4CC1-BFC6-CA309B41AD35}">
   <dimension ref="A1:I255"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2046,7 +2046,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="67"/>
@@ -2089,7 +2089,7 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" s="70"/>
       <c r="C5" s="71"/>
@@ -2113,7 +2113,7 @@
     </row>
     <row r="7" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="68" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B7" s="66"/>
       <c r="C7" s="67"/>
@@ -2243,7 +2243,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="65" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B19" s="66"/>
       <c r="C19" s="67"/>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="21" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="65" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B21" s="66"/>
       <c r="C21" s="67"/>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="29" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="65" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B29" s="66"/>
       <c r="C29" s="67"/>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="35" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" s="65" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B35" s="66"/>
       <c r="C35" s="67"/>
@@ -2452,7 +2452,7 @@
     </row>
     <row r="38" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="75" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B38" s="76"/>
       <c r="C38" s="77"/>
@@ -2477,7 +2477,7 @@
     </row>
     <row r="41" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A41" s="68" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B41" s="66"/>
       <c r="C41" s="67"/>
@@ -2714,7 +2714,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="68" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B17" s="66"/>
       <c r="C17" s="67"/>
@@ -2746,7 +2746,7 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="68" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B21" s="66"/>
       <c r="C21" s="67"/>
@@ -2775,7 +2775,7 @@
     </row>
     <row r="25" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="68" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B25" s="66"/>
       <c r="C25" s="67"/>
@@ -2884,8 +2884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD54838-E504-4CBA-8D4E-DD881A64EA8E}">
   <dimension ref="A1:I254"/>
   <sheetViews>
-    <sheetView topLeftCell="A144" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A178" sqref="A178:C178"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2907,7 +2907,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="B1" s="70"/>
       <c r="C1" s="71"/>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="72" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="B27" s="73"/>
       <c r="C27" s="74"/>
@@ -3187,7 +3187,7 @@
         <v>4191.5999999999995</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3211,7 +3211,7 @@
         <v>1538.8000000000002</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3248,7 +3248,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I33" s="5"/>
     </row>
@@ -3262,7 +3262,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3352,7 +3352,7 @@
         <v>167.67000000000002</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3418,19 +3418,19 @@
     </row>
     <row r="50" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A50" s="92" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B50" s="93"/>
       <c r="C50" s="93"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3674,19 +3674,19 @@
     </row>
     <row r="78" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A78" s="80" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B78" s="81"/>
       <c r="C78" s="81"/>
     </row>
     <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3919,19 +3919,19 @@
     </row>
     <row r="105" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" s="80" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B105" s="81"/>
       <c r="C105" s="81"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4164,19 +4164,19 @@
     </row>
     <row r="132" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A132" s="80" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B132" s="81"/>
       <c r="C132" s="81"/>
     </row>
     <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4371,19 +4371,19 @@
     </row>
     <row r="155" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A155" s="80" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B155" s="81"/>
       <c r="C155" s="81"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4578,19 +4578,19 @@
     </row>
     <row r="178" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A178" s="80" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B178" s="81"/>
       <c r="C178" s="81"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Introduced Miscellaneous Data as a Block in Statics Sheet.
</commit_message>
<xml_diff>
--- a/myStudies/RothConversion.xlsx
+++ b/myStudies/RothConversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkrat\git\MyStudiesRepo\myStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF858DC-FD5E-4AF1-B6FD-B674BF3CDF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8D2B1A-82AA-436D-9293-641DE03936FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" activeTab="2" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statics" sheetId="38" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="125">
   <si>
     <t>Description</t>
   </si>
@@ -422,6 +422,12 @@
   </si>
   <si>
     <t>Long-Term</t>
+  </si>
+  <si>
+    <t>Max Capital Gains Loss</t>
+  </si>
+  <si>
+    <t>Misc Data</t>
   </si>
 </sst>
 </file>
@@ -2094,10 +2100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8746EC-93A7-4CC1-BFC6-CA309B41AD35}">
-  <dimension ref="A1:I251"/>
+  <dimension ref="A1:I253"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2119,7 +2125,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickTop="1">
       <c r="A1" s="72" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="B1" s="73"/>
       <c r="C1" s="74"/>
@@ -2130,51 +2136,61 @@
         <v>45413</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="50">
+    <row r="2" spans="1:8">
+      <c r="A2" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="50">
         <v>45422</v>
       </c>
-      <c r="B2" s="50"/>
       <c r="C2" s="6"/>
       <c r="D2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickTop="1">
-      <c r="A3" s="72" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="74"/>
+      <c r="B3" s="63">
+        <v>2027</v>
+      </c>
+      <c r="C3" s="6"/>
       <c r="D3" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A4" s="63">
-        <v>2027</v>
-      </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="6"/>
+    <row r="4" spans="1:8">
+      <c r="A4" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="21">
+        <v>30700</v>
+      </c>
+      <c r="C4" s="19"/>
       <c r="D4" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickTop="1">
-      <c r="A5" s="76" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="78"/>
+    <row r="5" spans="1:8">
+      <c r="A5" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="43">
+        <v>174.7</v>
+      </c>
+      <c r="C5" s="44"/>
       <c r="D5" s="14" t="s">
         <v>53</v>
       </c>
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A6" s="25"/>
+      <c r="A6" s="64" t="s">
+        <v>123</v>
+      </c>
       <c r="B6" s="21">
-        <v>30700</v>
+        <v>3000</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="14" t="s">
@@ -2185,8 +2201,8 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A7" s="75" t="s">
-        <v>108</v>
+      <c r="A7" s="72" t="s">
+        <v>84</v>
       </c>
       <c r="B7" s="73"/>
       <c r="C7" s="74"/>
@@ -2198,428 +2214,411 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A8" s="42"/>
-      <c r="B8" s="43">
-        <v>174.7</v>
-      </c>
-      <c r="C8" s="44"/>
+    <row r="8" spans="1:8">
+      <c r="A8" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="50">
+        <v>19661</v>
+      </c>
+      <c r="C8" s="6"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickTop="1">
-      <c r="A9" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="74"/>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="25" t="s">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A9" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="50">
+        <v>20859</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickTop="1">
+      <c r="A10" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="73"/>
+      <c r="C10" s="74"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="51" t="s">
         <v>73</v>
-      </c>
-      <c r="B10" s="50">
-        <v>19661</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A11" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="50">
-        <v>20859</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A13" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickTop="1">
-      <c r="A12" s="72" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="73"/>
-      <c r="C12" s="74"/>
-      <c r="D12" t="s">
+    <row r="14" spans="1:8" ht="15.75" thickTop="1">
+      <c r="A14" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="73"/>
+      <c r="C14" s="74"/>
+      <c r="D14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="51" t="s">
+    <row r="15" spans="1:8">
+      <c r="A15" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="2">
         <v>73</v>
       </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="51" t="s">
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A16" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="2">
         <v>73</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="4" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A15" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4" t="s">
+    <row r="17" spans="1:4" ht="15.75" thickTop="1">
+      <c r="A17" s="72" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="73"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="4" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickTop="1">
-      <c r="A16" s="72" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="73"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="2">
-        <v>73</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1">
       <c r="A18" s="25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" s="2">
-        <v>73</v>
+        <v>17.2</v>
       </c>
       <c r="C18" s="6"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickTop="1">
       <c r="A19" s="72" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B19" s="73"/>
       <c r="C19" s="74"/>
       <c r="D19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="2">
-        <v>17.2</v>
+      <c r="B20" s="21">
+        <v>41925.5</v>
       </c>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A21" s="72" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="73"/>
-      <c r="C21" s="74"/>
+    <row r="21" spans="1:4">
+      <c r="A21" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="21">
+        <v>2082478.98</v>
+      </c>
+      <c r="C21" s="6"/>
       <c r="D21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A22" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="21">
+        <v>1049867.8400000001</v>
+      </c>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickTop="1">
+      <c r="A23" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="73"/>
+      <c r="C23" s="74"/>
+      <c r="D23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="25" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="21">
-        <v>41925.5</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="21">
-        <v>2082478.98</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A24" s="25" t="s">
-        <v>79</v>
-      </c>
       <c r="B24" s="21">
-        <v>1049867.8400000001</v>
+        <v>41925</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A25" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="73"/>
-      <c r="C25" s="74"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="21">
+        <v>2200000</v>
+      </c>
+      <c r="C25" s="6"/>
       <c r="D25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1">
       <c r="A26" s="25" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B26" s="21">
-        <v>41925</v>
+        <v>1009000</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="21">
-        <v>2200000</v>
-      </c>
-      <c r="C27" s="6"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickTop="1">
+      <c r="A27" s="72" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="73"/>
+      <c r="C27" s="74"/>
       <c r="D27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="25" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B28" s="21">
-        <v>1009000</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A29" s="72" t="s">
-        <v>119</v>
-      </c>
-      <c r="B29" s="73"/>
-      <c r="C29" s="74"/>
-      <c r="D29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30" s="21">
         <f>10*1487.9</f>
         <v>14879</v>
       </c>
-      <c r="C30" s="21"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A31" s="25" t="s">
+      <c r="C28" s="21"/>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A29" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B29" s="21">
         <f>12*2578.9</f>
         <v>30946.800000000003</v>
       </c>
+      <c r="C29" s="6"/>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickTop="1">
+      <c r="A30" s="72" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="73"/>
+      <c r="C30" s="74"/>
+      <c r="D30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="51" t="s">
+        <v>74</v>
+      </c>
       <c r="C31" s="6"/>
-      <c r="D31" s="45" t="s">
+      <c r="D31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A32" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickTop="1">
+      <c r="A33" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="73"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="45" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A32" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="73"/>
-      <c r="C32" s="74"/>
-      <c r="D32" s="46" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="25" t="s">
+    <row r="34" spans="1:6">
+      <c r="A34" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A34" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="B34" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickTop="1">
-      <c r="A35" s="72" t="s">
-        <v>114</v>
-      </c>
-      <c r="B35" s="73"/>
-      <c r="C35" s="74"/>
-      <c r="D35" s="49" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" s="21">
+      <c r="B34" s="21">
         <f>12*2578.1</f>
         <v>30937.199999999997</v>
       </c>
-      <c r="C36" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A35" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="21">
+        <f>71065.98-50692.01</f>
+        <v>20373.969999999994</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickTop="1">
+      <c r="A36" s="72" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="73"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="48" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1">
       <c r="A37" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="21">
-        <f>71065.98-50692.01</f>
-        <v>20373.969999999994</v>
+      <c r="B37" s="63">
+        <v>2025</v>
       </c>
       <c r="C37" s="6"/>
-      <c r="F37" s="4"/>
+      <c r="D37" s="49" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickTop="1">
-      <c r="A38" s="72" t="s">
-        <v>113</v>
+      <c r="A38" s="75" t="s">
+        <v>106</v>
       </c>
       <c r="B38" s="73"/>
       <c r="C38" s="74"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A39" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="B39" s="63">
-        <v>2025</v>
-      </c>
-      <c r="C39" s="6"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" thickTop="1">
-      <c r="A40" s="75" t="s">
-        <v>106</v>
-      </c>
-      <c r="B40" s="73"/>
-      <c r="C40" s="74"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="20" t="s">
+    <row r="39" spans="1:6">
+      <c r="A39" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="64">
+      <c r="B39" s="64">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A42" s="20" t="s">
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A40" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="64">
+      <c r="B40" s="64">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" thickTop="1">
-      <c r="A43" s="79" t="s">
+    <row r="41" spans="1:6" ht="15.75" thickTop="1">
+      <c r="A41" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="80"/>
-      <c r="C43" s="81"/>
-    </row>
-    <row r="49" spans="9:9" ht="15.75" customHeight="1"/>
-    <row r="52" spans="9:9">
-      <c r="I52" s="3"/>
-    </row>
-    <row r="53" spans="9:9">
-      <c r="I53" s="5"/>
-    </row>
+      <c r="B41" s="80"/>
+      <c r="C41" s="81"/>
+    </row>
+    <row r="51" spans="9:9" ht="15.75" customHeight="1"/>
     <row r="54" spans="9:9">
-      <c r="I54" s="5"/>
-    </row>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="9:9">
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="9:9">
+      <c r="I56" s="5"/>
+    </row>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
     <row r="147" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
     <row r="173" ht="15.75" customHeight="1"/>
-    <row r="178" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="182" spans="4:4">
-      <c r="D182" s="1"/>
-    </row>
-    <row r="187" spans="4:4">
-      <c r="D187" s="1"/>
-    </row>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="180" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="184" spans="4:4">
+      <c r="D184" s="1"/>
+    </row>
+    <row r="189" spans="4:4">
+      <c r="D189" s="1"/>
+    </row>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
+  <mergeCells count="13">
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A14:C14"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2628,10 +2627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFC4955-0F80-43F5-88A1-E586421548F7}">
-  <dimension ref="A1:I267"/>
+  <dimension ref="A1:I271"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:C32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2808,136 +2807,138 @@
       <c r="B20" s="22"/>
       <c r="C20" s="19"/>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A21" s="75" t="s">
-        <v>105</v>
-      </c>
-      <c r="B21" s="73"/>
-      <c r="C21" s="74"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="64">
-        <v>0</v>
-      </c>
-      <c r="B22" s="21">
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="64">
-        <v>0.5</v>
-      </c>
-      <c r="B23" s="21">
-        <v>44000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A24" s="64">
-        <v>0.85</v>
-      </c>
-      <c r="B24" s="21"/>
-    </row>
+    <row r="21" spans="1:3" ht="15.75" thickTop="1"/>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="25" spans="1:3" ht="15.75" thickTop="1">
       <c r="A25" s="75" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B25" s="73"/>
       <c r="C25" s="74"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="64">
-        <v>1</v>
-      </c>
-      <c r="B26" s="41">
-        <v>210000</v>
+        <v>0</v>
+      </c>
+      <c r="B26" s="21">
+        <v>32000</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="64">
-        <v>1.4</v>
-      </c>
-      <c r="B27" s="41">
-        <v>264000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>0.5</v>
+      </c>
+      <c r="B27" s="21">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1">
       <c r="A28" s="64">
-        <v>2</v>
-      </c>
-      <c r="B28" s="41">
-        <v>330000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="64">
-        <v>2.6</v>
-      </c>
-      <c r="B29" s="41">
-        <v>394000</v>
-      </c>
+        <v>0.85</v>
+      </c>
+      <c r="B28" s="21"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" thickTop="1">
+      <c r="A29" s="75" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="73"/>
+      <c r="C29" s="74"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="64">
+        <v>1</v>
+      </c>
+      <c r="B30" s="41">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="64">
+        <v>1.4</v>
+      </c>
+      <c r="B31" s="41">
+        <v>264000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="64">
+        <v>2</v>
+      </c>
+      <c r="B32" s="41">
+        <v>330000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="64">
+        <v>2.6</v>
+      </c>
+      <c r="B33" s="41">
+        <v>394000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="64">
         <v>3.2</v>
       </c>
-      <c r="B30" s="41">
+      <c r="B34" s="41">
         <v>750000</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A31" s="64">
+    <row r="35" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A35" s="64">
         <v>3.4</v>
       </c>
-      <c r="B31" s="41"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A32" s="79" t="s">
+      <c r="B35" s="41"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" thickTop="1">
+      <c r="A36" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="80"/>
-      <c r="C32" s="81"/>
-    </row>
-    <row r="44" spans="9:9">
-      <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="9:9">
-      <c r="I45" s="5"/>
-    </row>
-    <row r="46" spans="9:9">
-      <c r="I46" s="5"/>
-    </row>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="194" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="204" spans="4:4">
-      <c r="D204" s="1"/>
-    </row>
-    <row r="209" spans="4:4">
-      <c r="D209" s="1"/>
-    </row>
-    <row r="215" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="222" spans="4:4" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="81"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="9:9">
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="9:9">
+      <c r="I50" s="5"/>
+    </row>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="193" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="198" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="208" spans="4:4">
+      <c r="D208" s="1"/>
+    </row>
+    <row r="213" spans="4:4">
+      <c r="D213" s="1"/>
+    </row>
+    <row r="219" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A36:C36"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A29:C29"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2948,7 +2949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699D3255-6ECC-45F2-AB86-133EB1B0B627}">
   <dimension ref="A1:I248"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Rearranged Spreadsheet and revised CapitalGains Calcs.
</commit_message>
<xml_diff>
--- a/myStudies/RothConversion.xlsx
+++ b/myStudies/RothConversion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkrat\git\MyStudiesRepo\myStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8D2B1A-82AA-436D-9293-641DE03936FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997C9095-FC46-4D9F-82AB-2C629D25D389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="124">
   <si>
     <t>Description</t>
   </si>
@@ -286,15 +286,6 @@
     <t>Tax Brackets</t>
   </si>
   <si>
-    <t>Thomas 00</t>
-  </si>
-  <si>
-    <t>Thomas 01</t>
-  </si>
-  <si>
-    <t>Diem-Tran 00</t>
-  </si>
-  <si>
     <t>End Data</t>
   </si>
   <si>
@@ -373,9 +364,6 @@
     <t>Social Security AGI Tax Rates</t>
   </si>
   <si>
-    <t>Growth Rates</t>
-  </si>
-  <si>
     <t>Current Date</t>
   </si>
   <si>
@@ -409,9 +397,6 @@
     <t>Basis</t>
   </si>
   <si>
-    <t>Long/Total</t>
-  </si>
-  <si>
     <t>SSA</t>
   </si>
   <si>
@@ -427,7 +412,19 @@
     <t>Max Capital Gains Loss</t>
   </si>
   <si>
-    <t>Misc Data</t>
+    <t>Miscellaneous Data</t>
+  </si>
+  <si>
+    <t>% that's Long</t>
+  </si>
+  <si>
+    <t>Thomas-Inh</t>
+  </si>
+  <si>
+    <t>Thomas-R/O</t>
+  </si>
+  <si>
+    <t>Diem-Tran-TSP</t>
   </si>
 </sst>
 </file>
@@ -1494,7 +1491,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1646,7 +1643,15 @@
     <xf numFmtId="0" fontId="25" fillId="35" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="8" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" xfId="8" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="34" xfId="8" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="45" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1659,6 +1664,48 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="28" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1668,57 +1715,12 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="34" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="8" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" xfId="8" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="34" xfId="8" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="36" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1727,12 +1729,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="38" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -2103,7 +2099,7 @@
   <dimension ref="A1:I253"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A10" sqref="A10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2124,11 +2120,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickTop="1">
-      <c r="A1" s="72" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="74"/>
+      <c r="A1" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="76"/>
       <c r="D1" t="s">
         <v>62</v>
       </c>
@@ -2138,7 +2134,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="50" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B2" s="50">
         <v>45422</v>
@@ -2150,7 +2146,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="63" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B3" s="63">
         <v>2027</v>
@@ -2162,7 +2158,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B4" s="21">
         <v>30700</v>
@@ -2174,7 +2170,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="42" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B5" s="43">
         <v>174.7</v>
@@ -2185,9 +2181,9 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
+    <row r="6" spans="1:8">
       <c r="A6" s="64" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B6" s="21">
         <v>3000</v>
@@ -2200,12 +2196,13 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A7" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="74"/>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A7" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="64">
+        <v>0.05</v>
+      </c>
       <c r="D7" s="15" t="s">
         <v>52</v>
       </c>
@@ -2215,361 +2212,362 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="50">
-        <v>19661</v>
-      </c>
-      <c r="C8" s="6"/>
+      <c r="A8" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="64">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A9" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="50">
-        <v>20859</v>
+      <c r="A9" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="64">
+        <v>0.66666666666666663</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickTop="1">
-      <c r="A10" s="72" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="74"/>
+      <c r="A10" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="75"/>
+      <c r="C10" s="76"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="51" t="s">
         <v>73</v>
       </c>
+      <c r="B11" s="50">
+        <v>19661</v>
+      </c>
       <c r="C11" s="6"/>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A12" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="50">
+        <v>20859</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="6"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A13" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" t="s">
+    <row r="13" spans="1:8" ht="15.75" thickTop="1">
+      <c r="A13" s="74" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="75"/>
+      <c r="C13" s="76"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickTop="1">
-      <c r="A14" s="72" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="74"/>
-      <c r="D14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" s="2">
+        <v>122</v>
+      </c>
+      <c r="B15" s="51" t="s">
         <v>73</v>
       </c>
       <c r="C15" s="6"/>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1">
       <c r="A16" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="2">
+        <v>123</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickTop="1">
+      <c r="A17" s="74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="75"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="2">
         <v>73</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A17" s="72" t="s">
-        <v>101</v>
-      </c>
-      <c r="B17" s="73"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="4" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A18" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="2">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A19" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="2">
+        <v>73</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickTop="1">
+      <c r="A20" s="74" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="75"/>
+      <c r="C20" s="76"/>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A21" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="2">
         <v>17.2</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A19" s="72" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="74"/>
-      <c r="D19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="21">
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickTop="1">
+      <c r="A22" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="75"/>
+      <c r="C22" s="76"/>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="21">
         <v>41925.5</v>
       </c>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="21">
-        <v>2082478.98</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A22" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="21">
-        <v>1049867.8400000001</v>
-      </c>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A23" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="74"/>
-      <c r="D23" t="s">
-        <v>64</v>
-      </c>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="25" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="B24" s="21">
-        <v>41925</v>
+        <v>2082478.98</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1">
       <c r="A25" s="25" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="B25" s="21">
-        <v>2200000</v>
+        <v>1049867.8400000001</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickTop="1">
+      <c r="A26" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="75"/>
+      <c r="C26" s="76"/>
+      <c r="D26" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A26" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="21">
-        <v>1009000</v>
-      </c>
-      <c r="C26" s="6"/>
-      <c r="D26" t="s">
+    <row r="27" spans="1:4">
+      <c r="A27" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="21">
+        <v>41925</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A27" s="72" t="s">
-        <v>119</v>
-      </c>
-      <c r="B27" s="73"/>
-      <c r="C27" s="74"/>
-      <c r="D27" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="21">
+        <v>2200000</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A29" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="21">
+        <v>1009000</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickTop="1">
+      <c r="A30" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="75"/>
+      <c r="C30" s="76"/>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B31" s="21">
         <f>10*1487.9</f>
         <v>14879</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A29" s="25" t="s">
+      <c r="C31" s="21"/>
+      <c r="D31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A32" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="21">
+      <c r="B32" s="21">
         <f>12*2578.9</f>
         <v>30946.800000000003</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A30" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="73"/>
-      <c r="C30" s="74"/>
-      <c r="D30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B31" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" t="s">
+      <c r="C32" s="6"/>
+      <c r="D32" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A32" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="B32" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" s="6"/>
-    </row>
     <row r="33" spans="1:6" ht="15.75" thickTop="1">
-      <c r="A33" s="72" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33" s="73"/>
-      <c r="C33" s="74"/>
-      <c r="D33" s="45" t="s">
-        <v>55</v>
-      </c>
+      <c r="A33" s="74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="75"/>
+      <c r="C33" s="76"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" s="21">
+        <v>83</v>
+      </c>
+      <c r="B34" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A35" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickTop="1">
+      <c r="A36" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="75"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="21">
         <f>12*2578.1</f>
         <v>30937.199999999997</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="46" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A35" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="B35" s="21">
+      <c r="C37" s="6"/>
+      <c r="D37" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A38" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="21">
         <f>71065.98-50692.01</f>
         <v>20373.969999999994</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" thickTop="1">
-      <c r="A36" s="72" t="s">
-        <v>113</v>
-      </c>
-      <c r="B36" s="73"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A37" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="B37" s="63">
+      <c r="C38" s="6"/>
+      <c r="D38" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" thickTop="1">
+      <c r="A39" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="75"/>
+      <c r="C39" s="76"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A40" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="63">
         <v>2025</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="49" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" thickTop="1">
-      <c r="A38" s="75" t="s">
-        <v>106</v>
-      </c>
-      <c r="B38" s="73"/>
-      <c r="C38" s="74"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="64">
-        <v>0.05</v>
-      </c>
-      <c r="F39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A40" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="64">
-        <v>7.0000000000000007E-2</v>
-      </c>
+      <c r="C40" s="6"/>
+      <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickTop="1">
-      <c r="A41" s="79" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="80"/>
-      <c r="C41" s="81"/>
+      <c r="A41" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="72"/>
+      <c r="C41" s="73"/>
     </row>
     <row r="51" spans="9:9" ht="15.75" customHeight="1"/>
     <row r="54" spans="9:9">
@@ -2605,20 +2603,19 @@
     <row r="225" ht="15.75" customHeight="1"/>
     <row r="253" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A7:C7"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A26:C26"/>
     <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2651,11 +2648,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="74"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="76"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="64">
@@ -2719,12 +2716,12 @@
       <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A9" s="75" t="str">
+      <c r="A9" s="77" t="str">
         <f>_xlfn.CONCAT(A1," 2026")</f>
         <v>Tax Brackets 2026</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="74"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="76"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="64">
@@ -2776,11 +2773,11 @@
       <c r="C16" s="19"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A17" s="75" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" s="73"/>
-      <c r="C17" s="74"/>
+      <c r="A17" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="75"/>
+      <c r="C17" s="76"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="64">
@@ -2810,11 +2807,11 @@
     <row r="21" spans="1:3" ht="15.75" thickTop="1"/>
     <row r="24" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="25" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A25" s="75" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="73"/>
-      <c r="C25" s="74"/>
+      <c r="A25" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="75"/>
+      <c r="C25" s="76"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="64">
@@ -2839,11 +2836,11 @@
       <c r="B28" s="21"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A29" s="75" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="73"/>
-      <c r="C29" s="74"/>
+      <c r="A29" s="77" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="75"/>
+      <c r="C29" s="76"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="64">
@@ -2892,11 +2889,11 @@
       <c r="B35" s="41"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" thickTop="1">
-      <c r="A36" s="79" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="80"/>
-      <c r="C36" s="81"/>
+      <c r="A36" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="72"/>
+      <c r="C36" s="73"/>
     </row>
     <row r="48" spans="1:9">
       <c r="I48" s="3"/>
@@ -2947,10 +2944,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699D3255-6ECC-45F2-AB86-133EB1B0B627}">
-  <dimension ref="A1:I248"/>
+  <dimension ref="A1:I247"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2971,19 +2968,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A1" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="78"/>
+      <c r="A1" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="93"/>
+      <c r="C1" s="94"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="28" t="str">
-        <f t="shared" ref="A2:A7" si="0">A49</f>
+        <f t="shared" ref="A2:A7" si="0">A48</f>
         <v>- Ordinary Dividends</v>
       </c>
       <c r="B2" s="29">
-        <f t="shared" ref="B2:B17" si="1">SUMIFS(C$45:C$125,A$45:A$125,A2)</f>
+        <f t="shared" ref="B2:B17" si="1">SUMIFS(C$44:C$124,A$44:A$124,A2)</f>
         <v>4191.6099999999997</v>
       </c>
       <c r="C2" s="6"/>
@@ -3045,7 +3042,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="28" t="str">
-        <f>A57</f>
+        <f>A56</f>
         <v>Tax-Exempt Income</v>
       </c>
       <c r="B8" s="29">
@@ -3056,7 +3053,7 @@
     </row>
     <row r="9" spans="1:3" ht="16.5" customHeight="1">
       <c r="A9" s="28" t="str">
-        <f t="shared" ref="A9:A14" si="2">A61</f>
+        <f t="shared" ref="A9:A14" si="2">A60</f>
         <v>Net Short-Term</v>
       </c>
       <c r="B9" s="29">
@@ -3122,7 +3119,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="28" t="str">
-        <f>A69</f>
+        <f>A68</f>
         <v>Margin Interest Paid</v>
       </c>
       <c r="B15" s="29">
@@ -3133,7 +3130,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="28" t="str">
-        <f>A70</f>
+        <f>A69</f>
         <v>Option Sales</v>
       </c>
       <c r="B16" s="29">
@@ -3144,7 +3141,7 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="28" t="str">
-        <f>A71</f>
+        <f>A70</f>
         <v>Return of Principal</v>
       </c>
       <c r="B17" s="29">
@@ -3154,26 +3151,26 @@
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickTop="1">
-      <c r="A18" s="79" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18" s="80"/>
-      <c r="C18" s="81"/>
+      <c r="A18" s="71" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="72"/>
+      <c r="C18" s="73"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="28" t="str">
-        <f>A131</f>
+        <f>A130</f>
         <v>- Non-Qualified Dividends</v>
       </c>
       <c r="B19" s="29">
-        <f t="shared" ref="B19:B33" si="3">SUMIFS(C$127:C$194,A$127:A$194,A19)</f>
+        <f t="shared" ref="B19:B33" si="3">SUMIFS(C$126:C$193,A$126:A$193,A19)</f>
         <v>2652.8</v>
       </c>
       <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="28" t="str">
-        <f>A132</f>
+        <f>A131</f>
         <v>- Qualified Dividends</v>
       </c>
       <c r="B20" s="29">
@@ -3184,7 +3181,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="28" t="str">
-        <f>A133</f>
+        <f>A132</f>
         <v>- Section 897 Ordinary Dividends</v>
       </c>
       <c r="B21" s="29">
@@ -3195,7 +3192,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="28" t="str">
-        <f>A134</f>
+        <f>A133</f>
         <v>- Section 199A Dividends</v>
       </c>
       <c r="B22" s="29">
@@ -3207,7 +3204,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="28" t="str">
-        <f t="shared" ref="A23:A28" si="4">A136</f>
+        <f t="shared" ref="A23:A28" si="4">A135</f>
         <v>- Unrecaptured Section 1250 Capital Gains</v>
       </c>
       <c r="B23" s="29">
@@ -3274,7 +3271,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="28" t="str">
-        <f>A143</f>
+        <f>A142</f>
         <v>Investment Expenses</v>
       </c>
       <c r="B29" s="29">
@@ -3285,7 +3282,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="28" t="str">
-        <f>A144</f>
+        <f>A143</f>
         <v>Foreign Tax Paid</v>
       </c>
       <c r="B30" s="29">
@@ -3296,7 +3293,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="28" t="str">
-        <f>A146</f>
+        <f>A145</f>
         <v>Cash Liquidation Distributions</v>
       </c>
       <c r="B31" s="29">
@@ -3307,7 +3304,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="28" t="str">
-        <f>A147</f>
+        <f>A146</f>
         <v>Non-cash Liquidation Distributions</v>
       </c>
       <c r="B32" s="29">
@@ -3318,7 +3315,7 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1">
       <c r="A33" s="28" t="str">
-        <f>A148</f>
+        <f>A147</f>
         <v>Total Tax Exempt Interest Dividends</v>
       </c>
       <c r="B33" s="29">
@@ -3328,15 +3325,15 @@
       <c r="C33" s="6"/>
     </row>
     <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A34" s="96" t="s">
-        <v>120</v>
-      </c>
-      <c r="B34" s="97"/>
-      <c r="C34" s="98"/>
+      <c r="A34" s="97" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="98"/>
+      <c r="C34" s="99"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickTop="1">
       <c r="A35" s="30" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B35" s="31">
         <v>-10950</v>
@@ -3345,7 +3342,7 @@
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1">
       <c r="A36" s="18" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B36" s="22">
         <v>-17755</v>
@@ -3353,15 +3350,15 @@
       <c r="C36" s="23"/>
     </row>
     <row r="37" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A37" s="79" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="80"/>
-      <c r="C37" s="81"/>
+      <c r="A37" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="72"/>
+      <c r="C37" s="73"/>
     </row>
     <row r="38" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
       <c r="A38" s="28" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B38" s="31">
         <v>792816.17999999993</v>
@@ -3370,95 +3367,97 @@
     </row>
     <row r="39" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
       <c r="A39" s="28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B39" s="31">
         <v>454641.68999999994</v>
       </c>
       <c r="C39" s="6"/>
     </row>
-    <row r="40" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A40" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" s="71">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C40" s="6"/>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A41" s="79" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="80"/>
-      <c r="C41" s="81"/>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A42" s="24"/>
-    </row>
-    <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A43" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="B43" s="80"/>
-      <c r="C43" s="81"/>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A44" s="84" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" s="85"/>
-      <c r="C44" s="85"/>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A46" s="39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A47" s="86" t="s">
+    <row r="40" spans="1:3" ht="15.75" thickTop="1">
+      <c r="A40" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="72"/>
+      <c r="C40" s="73"/>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A41" s="24"/>
+    </row>
+    <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A42" s="71" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="72"/>
+      <c r="C42" s="73"/>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" thickTop="1">
+      <c r="A43" s="95" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="96"/>
+      <c r="C43" s="96"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A45" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A46" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="86"/>
-      <c r="C47" s="52">
+      <c r="B46" s="82"/>
+      <c r="C46" s="52">
         <v>2148.12</v>
       </c>
     </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="53"/>
+    </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" s="8" t="s">
+      <c r="A48" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="84"/>
+      <c r="C48" s="54">
+        <v>2148.12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A49" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="86"/>
+      <c r="C49" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A50" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="53"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="87" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" s="88"/>
-      <c r="C49" s="54">
-        <v>2148.12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A50" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" s="90"/>
-      <c r="C50" s="55">
+      <c r="C50" s="56">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1">
       <c r="A51" s="35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>3</v>
@@ -3469,7 +3468,7 @@
     </row>
     <row r="52" spans="1:3" ht="15.75" thickBot="1">
       <c r="A52" s="35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>3</v>
@@ -3480,7 +3479,7 @@
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1">
       <c r="A53" s="35" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>3</v>
@@ -3490,28 +3489,28 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A54" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="9" t="s">
+      <c r="A54" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="82"/>
+      <c r="C54" s="52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A55" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C54" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A55" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="B55" s="86"/>
-      <c r="C55" s="52">
+      <c r="C55" s="56">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1">
       <c r="A56" s="35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>3</v>
@@ -3521,64 +3520,64 @@
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A57" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B57" s="9" t="s">
+      <c r="A57" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="82"/>
+      <c r="C57" s="52">
+        <v>2148.12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A58" s="87"/>
+      <c r="B58" s="87"/>
+      <c r="C58" s="88"/>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A59" s="82" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="82"/>
+      <c r="C59" s="52">
+        <v>9919.7099999999991</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A60" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A58" s="86" t="s">
-        <v>12</v>
-      </c>
-      <c r="B58" s="86"/>
-      <c r="C58" s="52">
-        <v>2148.12</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A59" s="82"/>
-      <c r="B59" s="82"/>
-      <c r="C59" s="83"/>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A60" s="86" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="86"/>
-      <c r="C60" s="52">
-        <v>9919.7099999999991</v>
+      <c r="C60" s="56">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" thickBot="1">
       <c r="A61" s="35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C61" s="56">
-        <v>0</v>
+        <v>9919.7099999999991</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A62" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="B62" s="7" t="s">
+      <c r="A62" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="56">
-        <v>9919.7099999999991</v>
+      <c r="C62" s="57">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1">
       <c r="A63" s="36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>3</v>
@@ -3589,7 +3588,7 @@
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1">
       <c r="A64" s="36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>3</v>
@@ -3600,7 +3599,7 @@
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1">
       <c r="A65" s="36" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B65" s="10" t="s">
         <v>3</v>
@@ -3610,111 +3609,111 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A66" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" s="10" t="s">
+      <c r="A66" s="87"/>
+      <c r="B66" s="87"/>
+      <c r="C66" s="88"/>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A67" s="82" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" s="82"/>
+      <c r="C67" s="89"/>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" s="91"/>
+      <c r="C68" s="58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" s="84"/>
+      <c r="C69" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A70" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" s="11"/>
+      <c r="C70" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" thickTop="1">
+      <c r="A71" s="80" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71" s="81"/>
+      <c r="C71" s="81"/>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A72" s="38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A73" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A74" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="82"/>
+      <c r="C74" s="52">
+        <v>636.94000000000005</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A67" s="82"/>
-      <c r="B67" s="82"/>
-      <c r="C67" s="83"/>
-    </row>
-    <row r="68" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A68" s="86" t="s">
-        <v>20</v>
-      </c>
-      <c r="B68" s="86"/>
-      <c r="C68" s="91"/>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="92" t="s">
-        <v>21</v>
-      </c>
-      <c r="B69" s="93"/>
-      <c r="C69" s="58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="87" t="s">
-        <v>22</v>
-      </c>
-      <c r="B70" s="88"/>
-      <c r="C70" s="54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A71" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A72" s="94" t="s">
-        <v>94</v>
-      </c>
-      <c r="B72" s="95"/>
-      <c r="C72" s="95"/>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A73" s="38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A74" s="39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A75" s="86" t="s">
-        <v>1</v>
-      </c>
-      <c r="B75" s="86"/>
-      <c r="C75" s="52">
+      <c r="C75" s="53"/>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" s="84"/>
+      <c r="C76" s="54">
         <v>636.94000000000005</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B76" s="8" t="s">
+    <row r="77" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A77" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="86"/>
+      <c r="C77" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A78" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="53"/>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="87" t="s">
-        <v>4</v>
-      </c>
-      <c r="B77" s="88"/>
-      <c r="C77" s="54">
-        <v>636.94000000000005</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A78" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="B78" s="90"/>
-      <c r="C78" s="55">
+      <c r="C78" s="56">
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="15.75" thickBot="1">
       <c r="A79" s="35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>3</v>
@@ -3725,7 +3724,7 @@
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1">
       <c r="A80" s="35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>3</v>
@@ -3735,28 +3734,28 @@
       </c>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A81" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B81" s="9" t="s">
+      <c r="A81" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="B81" s="82"/>
+      <c r="C81" s="52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A82" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A82" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="B82" s="86"/>
-      <c r="C82" s="52">
+      <c r="C82" s="56">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1">
       <c r="A83" s="35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B83" s="9" t="s">
         <v>3</v>
@@ -3766,64 +3765,64 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A84" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B84" s="9" t="s">
+      <c r="A84" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" s="82"/>
+      <c r="C84" s="52">
+        <v>636.94000000000005</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A85" s="87"/>
+      <c r="B85" s="87"/>
+      <c r="C85" s="88"/>
+    </row>
+    <row r="86" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A86" s="82" t="s">
+        <v>13</v>
+      </c>
+      <c r="B86" s="82"/>
+      <c r="C86" s="59">
+        <v>-345.84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A87" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C84" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A85" s="86" t="s">
-        <v>12</v>
-      </c>
-      <c r="B85" s="86"/>
-      <c r="C85" s="52">
-        <v>636.94000000000005</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A86" s="82"/>
-      <c r="B86" s="82"/>
-      <c r="C86" s="83"/>
-    </row>
-    <row r="87" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A87" s="86" t="s">
-        <v>13</v>
-      </c>
-      <c r="B87" s="86"/>
-      <c r="C87" s="59">
-        <v>-345.84</v>
+      <c r="C87" s="56">
+        <v>-343.15</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15.75" thickBot="1">
       <c r="A88" s="35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C88" s="56">
-        <v>-343.15</v>
+        <v>-2.69</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A89" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="B89" s="7" t="s">
+      <c r="A89" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C89" s="56">
-        <v>-2.69</v>
+      <c r="C89" s="57">
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1">
       <c r="A90" s="36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B90" s="10" t="s">
         <v>3</v>
@@ -3834,7 +3833,7 @@
     </row>
     <row r="91" spans="1:3" ht="15.75" thickBot="1">
       <c r="A91" s="36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B91" s="10" t="s">
         <v>3</v>
@@ -3843,9 +3842,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="15.75" thickBot="1">
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A92" s="36" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B92" s="10" t="s">
         <v>3</v>
@@ -3854,112 +3853,112 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A93" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B93" s="10" t="s">
+    <row r="93" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A93" s="87"/>
+      <c r="B93" s="87"/>
+      <c r="C93" s="88"/>
+    </row>
+    <row r="94" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A94" s="82" t="s">
+        <v>20</v>
+      </c>
+      <c r="B94" s="82"/>
+      <c r="C94" s="89"/>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95" s="91"/>
+      <c r="C95" s="58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="B96" s="84"/>
+      <c r="C96" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A97" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B97" s="11"/>
+      <c r="C97" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" thickTop="1">
+      <c r="A98" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="B98" s="81"/>
+      <c r="C98" s="81"/>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A100" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A101" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="B101" s="82"/>
+      <c r="C101" s="52">
+        <v>1406.55</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B102" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C93" s="57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A94" s="82"/>
-      <c r="B94" s="82"/>
-      <c r="C94" s="83"/>
-    </row>
-    <row r="95" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A95" s="86" t="s">
-        <v>20</v>
-      </c>
-      <c r="B95" s="86"/>
-      <c r="C95" s="91"/>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" s="92" t="s">
-        <v>21</v>
-      </c>
-      <c r="B96" s="93"/>
-      <c r="C96" s="58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" s="87" t="s">
-        <v>22</v>
-      </c>
-      <c r="B97" s="88"/>
-      <c r="C97" s="54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A98" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A99" s="94" t="s">
-        <v>93</v>
-      </c>
-      <c r="B99" s="95"/>
-      <c r="C99" s="95"/>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" s="38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A101" s="39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A102" s="86" t="s">
-        <v>1</v>
-      </c>
-      <c r="B102" s="86"/>
-      <c r="C102" s="52">
+      <c r="C102" s="53"/>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103" s="84"/>
+      <c r="C103" s="54">
         <v>1406.55</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
-      <c r="A103" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B103" s="8" t="s">
+    <row r="104" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A104" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" s="86"/>
+      <c r="C104" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A105" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C103" s="53"/>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" s="87" t="s">
-        <v>4</v>
-      </c>
-      <c r="B104" s="88"/>
-      <c r="C104" s="54">
-        <v>1406.55</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A105" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="B105" s="90"/>
-      <c r="C105" s="55">
+      <c r="C105" s="56">
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15.75" thickBot="1">
       <c r="A106" s="35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B106" s="9" t="s">
         <v>3</v>
@@ -3970,7 +3969,7 @@
     </row>
     <row r="107" spans="1:3" ht="15.75" thickBot="1">
       <c r="A107" s="35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B107" s="9" t="s">
         <v>3</v>
@@ -3980,95 +3979,95 @@
       </c>
     </row>
     <row r="108" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A108" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B108" s="9" t="s">
+      <c r="A108" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="B108" s="82"/>
+      <c r="C108" s="52">
+        <v>15.05</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A109" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B109" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C108" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A109" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="B109" s="86"/>
-      <c r="C109" s="52">
+      <c r="C109" s="56">
         <v>15.05</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15.75" thickBot="1">
       <c r="A110" s="35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B110" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C110" s="56">
-        <v>15.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A111" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B111" s="9" t="s">
+      <c r="A111" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="B111" s="82"/>
+      <c r="C111" s="52">
+        <v>1421.6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A112" s="87"/>
+      <c r="B112" s="87"/>
+      <c r="C112" s="88"/>
+    </row>
+    <row r="113" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A113" s="82" t="s">
+        <v>13</v>
+      </c>
+      <c r="B113" s="82"/>
+      <c r="C113" s="59">
+        <v>-1352.29</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A114" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B114" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C111" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A112" s="86" t="s">
-        <v>12</v>
-      </c>
-      <c r="B112" s="86"/>
-      <c r="C112" s="52">
-        <v>1421.6</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A113" s="82"/>
-      <c r="B113" s="82"/>
-      <c r="C113" s="83"/>
-    </row>
-    <row r="114" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A114" s="86" t="s">
-        <v>13</v>
-      </c>
-      <c r="B114" s="86"/>
-      <c r="C114" s="59">
-        <v>-1352.29</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="15.75" thickBot="1">
+      <c r="C114" s="56">
+        <v>-1292.49</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A115" s="35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C115" s="56">
-        <v>-1292.49</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A116" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="B116" s="7" t="s">
+        <v>-59.8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A116" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B116" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C116" s="56">
-        <v>-59.8</v>
+      <c r="C116" s="57">
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="15.75" thickBot="1">
       <c r="A117" s="36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B117" s="10" t="s">
         <v>3</v>
@@ -4079,7 +4078,7 @@
     </row>
     <row r="118" spans="1:3" ht="15.75" thickBot="1">
       <c r="A118" s="36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B118" s="10" t="s">
         <v>3</v>
@@ -4090,7 +4089,7 @@
     </row>
     <row r="119" spans="1:3" ht="15.75" thickBot="1">
       <c r="A119" s="36" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B119" s="10" t="s">
         <v>3</v>
@@ -4100,113 +4099,111 @@
       </c>
     </row>
     <row r="120" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A120" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B120" s="10" t="s">
+      <c r="A120" s="87"/>
+      <c r="B120" s="87"/>
+      <c r="C120" s="88"/>
+    </row>
+    <row r="121" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A121" s="82" t="s">
+        <v>20</v>
+      </c>
+      <c r="B121" s="82"/>
+      <c r="C121" s="89"/>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B122" s="91"/>
+      <c r="C122" s="58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="B123" s="84"/>
+      <c r="C123" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A124" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B124" s="11"/>
+      <c r="C124" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="15.75" thickTop="1">
+      <c r="A125" s="80" t="s">
+        <v>94</v>
+      </c>
+      <c r="B125" s="81"/>
+      <c r="C125" s="81"/>
+    </row>
+    <row r="126" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A126" s="38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A127" s="39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A128" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B128" s="79"/>
+      <c r="C128" s="60" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A129" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B129" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C120" s="57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A121" s="82"/>
-      <c r="B121" s="82"/>
-      <c r="C121" s="83"/>
-    </row>
-    <row r="122" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A122" s="86" t="s">
-        <v>20</v>
-      </c>
-      <c r="B122" s="86"/>
-      <c r="C122" s="91"/>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" s="92" t="s">
-        <v>21</v>
-      </c>
-      <c r="B123" s="93"/>
-      <c r="C123" s="58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" s="87" t="s">
-        <v>22</v>
-      </c>
-      <c r="B124" s="88"/>
-      <c r="C124" s="54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A125" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B125" s="11"/>
-      <c r="C125" s="55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A126" s="94" t="s">
-        <v>97</v>
-      </c>
-      <c r="B126" s="95"/>
-      <c r="C126" s="95"/>
-    </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A127" s="38" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A128" s="39" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A129" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="B129" s="100"/>
-      <c r="C129" s="60" t="s">
-        <v>25</v>
+      <c r="C129" s="61">
+        <v>2148.12</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="15.75" thickBot="1">
       <c r="A130" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>3</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B130" s="12"/>
       <c r="C130" s="61">
-        <v>2148.12</v>
+        <v>1176.92</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="15.75" thickBot="1">
       <c r="A131" s="37" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B131" s="12"/>
       <c r="C131" s="61">
-        <v>1176.92</v>
+        <v>971.2</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="15.75" thickBot="1">
       <c r="A132" s="37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B132" s="12"/>
-      <c r="C132" s="61">
-        <v>971.2</v>
+      <c r="C132" s="62" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15.75" thickBot="1">
       <c r="A133" s="37" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B133" s="12"/>
       <c r="C133" s="62" t="s">
@@ -4215,27 +4212,27 @@
     </row>
     <row r="134" spans="1:3" ht="15.75" thickBot="1">
       <c r="A134" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B134" s="12"/>
-      <c r="C134" s="62" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C134" s="61">
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1">
       <c r="A135" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B135" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C135" s="61">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="B135" s="12"/>
+      <c r="C135" s="62" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="15.75" thickBot="1">
       <c r="A136" s="37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B136" s="12"/>
       <c r="C136" s="62" t="s">
@@ -4244,7 +4241,7 @@
     </row>
     <row r="137" spans="1:3" ht="15.75" thickBot="1">
       <c r="A137" s="37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B137" s="12"/>
       <c r="C137" s="62" t="s">
@@ -4253,7 +4250,7 @@
     </row>
     <row r="138" spans="1:3" ht="15.75" thickBot="1">
       <c r="A138" s="37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B138" s="12"/>
       <c r="C138" s="62" t="s">
@@ -4262,25 +4259,27 @@
     </row>
     <row r="139" spans="1:3" ht="15.75" thickBot="1">
       <c r="A139" s="37" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B139" s="12"/>
       <c r="C139" s="62" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="15.75" thickBot="1">
+    <row r="140" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A140" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="B140" s="12"/>
-      <c r="C140" s="62" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C140" s="61">
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A141" s="37" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B141" s="7" t="s">
         <v>3</v>
@@ -4289,131 +4288,129 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+    <row r="142" spans="1:3" ht="15.75" thickBot="1">
       <c r="A142" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B142" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B142" s="12"/>
+      <c r="C142" s="61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A143" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B143" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C142" s="61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A143" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B143" s="12"/>
       <c r="C143" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+    <row r="144" spans="1:3" ht="15.75" thickBot="1">
       <c r="A144" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B144" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C144" s="61">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="B144" s="12"/>
+      <c r="C144" s="62" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" thickBot="1">
       <c r="A145" s="37" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B145" s="12"/>
-      <c r="C145" s="62" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="15.75" thickBot="1">
+      <c r="C145" s="61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A146" s="37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B146" s="12"/>
       <c r="C146" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+    <row r="147" spans="1:3" ht="15.75" thickBot="1">
       <c r="A147" s="37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B147" s="12"/>
       <c r="C147" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A148" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B148" s="12"/>
-      <c r="C148" s="61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A149" s="94" t="s">
-        <v>98</v>
-      </c>
-      <c r="B149" s="95"/>
-      <c r="C149" s="95"/>
-    </row>
-    <row r="150" spans="1:3">
-      <c r="A150" s="38" t="s">
+    <row r="148" spans="1:3" ht="15.75" thickTop="1">
+      <c r="A148" s="80" t="s">
         <v>95</v>
       </c>
+      <c r="B148" s="81"/>
+      <c r="C148" s="81"/>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A150" s="39" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="151" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A151" s="39" t="s">
-        <v>96</v>
+      <c r="A151" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B151" s="79"/>
+      <c r="C151" s="60" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A152" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="B152" s="100"/>
-      <c r="C152" s="60" t="s">
-        <v>25</v>
+      <c r="A152" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C152" s="61">
+        <v>636.92999999999995</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="15.75" thickBot="1">
       <c r="A153" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B153" s="7" t="s">
-        <v>3</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B153" s="12"/>
       <c r="C153" s="61">
-        <v>636.92999999999995</v>
+        <v>69.33</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="15.75" thickBot="1">
       <c r="A154" s="37" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B154" s="12"/>
       <c r="C154" s="61">
-        <v>69.33</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="15.75" thickBot="1">
+        <v>567.6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A155" s="37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B155" s="12"/>
-      <c r="C155" s="61">
-        <v>567.6</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="C155" s="62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="15.75" thickBot="1">
       <c r="A156" s="37" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B156" s="12"/>
       <c r="C156" s="62" t="s">
@@ -4422,27 +4419,27 @@
     </row>
     <row r="157" spans="1:3" ht="15.75" thickBot="1">
       <c r="A157" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B157" s="12"/>
-      <c r="C157" s="62" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C157" s="61">
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="15.75" thickBot="1">
       <c r="A158" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B158" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C158" s="61">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="B158" s="12"/>
+      <c r="C158" s="62" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="15.75" thickBot="1">
       <c r="A159" s="37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B159" s="12"/>
       <c r="C159" s="62" t="s">
@@ -4451,7 +4448,7 @@
     </row>
     <row r="160" spans="1:3" ht="15.75" thickBot="1">
       <c r="A160" s="37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B160" s="12"/>
       <c r="C160" s="62" t="s">
@@ -4460,7 +4457,7 @@
     </row>
     <row r="161" spans="1:3" ht="15.75" thickBot="1">
       <c r="A161" s="37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B161" s="12"/>
       <c r="C161" s="62" t="s">
@@ -4469,7 +4466,7 @@
     </row>
     <row r="162" spans="1:3" ht="15.75" thickBot="1">
       <c r="A162" s="37" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B162" s="12"/>
       <c r="C162" s="62" t="s">
@@ -4478,16 +4475,18 @@
     </row>
     <row r="163" spans="1:3" ht="15.75" thickBot="1">
       <c r="A163" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="B163" s="12"/>
-      <c r="C163" s="62" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="B163" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C163" s="61">
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="15.75" thickBot="1">
       <c r="A164" s="37" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B164" s="7" t="s">
         <v>3</v>
@@ -4498,129 +4497,127 @@
     </row>
     <row r="165" spans="1:3" ht="15.75" thickBot="1">
       <c r="A165" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B165" s="7" t="s">
-        <v>3</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B165" s="12"/>
       <c r="C165" s="61">
         <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="15.75" thickBot="1">
       <c r="A166" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B166" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="B166" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="C166" s="61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="15.75" thickBot="1">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A167" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B167" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C167" s="61">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+        <v>46</v>
+      </c>
+      <c r="B167" s="12"/>
+      <c r="C167" s="62" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="15.75" thickBot="1">
       <c r="A168" s="37" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B168" s="12"/>
-      <c r="C168" s="62" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="15.75" thickBot="1">
+      <c r="C168" s="61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A169" s="37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B169" s="12"/>
       <c r="C169" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+    <row r="170" spans="1:3" ht="15.75" thickBot="1">
       <c r="A170" s="37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B170" s="12"/>
       <c r="C170" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A171" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B171" s="12"/>
-      <c r="C171" s="61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A172" s="94" t="s">
-        <v>99</v>
-      </c>
-      <c r="B172" s="95"/>
-      <c r="C172" s="95"/>
-    </row>
-    <row r="173" spans="1:3">
-      <c r="A173" s="38" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A174" s="39" t="s">
+    <row r="171" spans="1:3" ht="15.75" thickTop="1">
+      <c r="A171" s="80" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A175" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="B175" s="100"/>
-      <c r="C175" s="60" t="s">
+      <c r="B171" s="81"/>
+      <c r="C171" s="81"/>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A173" s="39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A174" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B174" s="79"/>
+      <c r="C174" s="60" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A175" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C175" s="61">
+        <v>1406.55</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="15.75" thickBot="1">
       <c r="A176" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B176" s="7" t="s">
-        <v>3</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B176" s="12"/>
       <c r="C176" s="61">
         <v>1406.55</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15.75" thickBot="1">
       <c r="A177" s="37" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B177" s="12"/>
       <c r="C177" s="61">
-        <v>1406.55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15.75" thickBot="1">
       <c r="A178" s="37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B178" s="12"/>
-      <c r="C178" s="61">
-        <v>0</v>
+      <c r="C178" s="62" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15.75" thickBot="1">
       <c r="A179" s="37" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B179" s="12"/>
       <c r="C179" s="62" t="s">
@@ -4629,27 +4626,27 @@
     </row>
     <row r="180" spans="1:4" ht="15.75" thickBot="1">
       <c r="A180" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B180" s="12"/>
-      <c r="C180" s="62" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="B180" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C180" s="61">
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15.75" thickBot="1">
       <c r="A181" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B181" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C181" s="61">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="B181" s="12"/>
+      <c r="C181" s="62" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="15.75" thickBot="1">
       <c r="A182" s="37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B182" s="12"/>
       <c r="C182" s="62" t="s">
@@ -4658,7 +4655,7 @@
     </row>
     <row r="183" spans="1:4" ht="15.75" thickBot="1">
       <c r="A183" s="37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B183" s="12"/>
       <c r="C183" s="62" t="s">
@@ -4667,87 +4664,87 @@
     </row>
     <row r="184" spans="1:4" ht="15.75" thickBot="1">
       <c r="A184" s="37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B184" s="12"/>
       <c r="C184" s="62" t="s">
         <v>35</v>
       </c>
+      <c r="D184" s="1"/>
     </row>
     <row r="185" spans="1:4" ht="15.75" thickBot="1">
       <c r="A185" s="37" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B185" s="12"/>
       <c r="C185" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="D185" s="1"/>
     </row>
     <row r="186" spans="1:4" ht="15.75" thickBot="1">
       <c r="A186" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="B186" s="12"/>
-      <c r="C186" s="62" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="B186" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C186" s="61">
+        <v>15.05</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="15.75" thickBot="1">
       <c r="A187" s="37" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B187" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C187" s="61">
-        <v>15.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="15.75" thickBot="1">
       <c r="A188" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B188" s="7" t="s">
-        <v>3</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B188" s="12"/>
       <c r="C188" s="61">
         <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="15.75" thickBot="1">
       <c r="A189" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B189" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="B189" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="C189" s="61">
-        <v>0</v>
-      </c>
+        <v>167.33</v>
+      </c>
+      <c r="D189" s="1"/>
     </row>
     <row r="190" spans="1:4" ht="15.75" thickBot="1">
       <c r="A190" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B190" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C190" s="61">
-        <v>167.33</v>
-      </c>
-      <c r="D190" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="B190" s="12"/>
+      <c r="C190" s="62" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="191" spans="1:4" ht="15.75" thickBot="1">
       <c r="A191" s="37" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B191" s="12"/>
-      <c r="C191" s="62" t="s">
-        <v>51</v>
+      <c r="C191" s="61">
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="15.75" thickBot="1">
       <c r="A192" s="37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B192" s="12"/>
       <c r="C192" s="61">
@@ -4756,135 +4753,126 @@
     </row>
     <row r="193" spans="1:3" ht="15.75" thickBot="1">
       <c r="A193" s="37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B193" s="12"/>
       <c r="C193" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A194" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B194" s="12"/>
-      <c r="C194" s="61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A195" s="26"/>
-      <c r="B195" s="27"/>
-      <c r="C195" s="26"/>
-    </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="194" spans="1:3" ht="15.75" thickTop="1">
+      <c r="A194" s="26"/>
+      <c r="B194" s="27"/>
+      <c r="C194" s="26"/>
+    </row>
+    <row r="195" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="202" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A149:C149"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A172:C172"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A94:C94"/>
-    <mergeCell ref="A95:C95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="A126:C126"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A113:C113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A121:C121"/>
-    <mergeCell ref="A122:C122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A58:C58"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A42:C42"/>
     <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A48:B48"/>
     <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A57:B57"/>
     <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A125:C125"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:C112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A120:C120"/>
+    <mergeCell ref="A121:C121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A98:C98"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="A94:C94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A148:C148"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="A171:C171"/>
+    <mergeCell ref="A174:B174"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B48" r:id="rId1" tooltip="Details for Ordinary Dividends and Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=X82865374&amp;TRS_TRAN_TYPE=1099-DIV&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=1&amp;txs=B" xr:uid="{1CD51B58-6A11-4DC5-8A80-9CCAEEF0E29C}"/>
-    <hyperlink ref="B51" r:id="rId2" tooltip="Details for Interest Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=X82865374&amp;TRS_TRAN_TYPE=1099-INT&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=2&amp;txs=C" xr:uid="{1E164B20-4BC7-4A31-89A0-25B5A2BDD0DC}"/>
-    <hyperlink ref="B52" r:id="rId3" tooltip="Details for Miscellaneous Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=X82865374&amp;TRS_TRAN_TYPE=1099-MISC&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=3&amp;txs=D" xr:uid="{0E88321C-3E19-484D-AC02-F09F9943D234}"/>
-    <hyperlink ref="B53" r:id="rId4" tooltip="Details for Original Issue Discount" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=X82865374&amp;SELECTED_YEAR_IND=0&amp;TRS_TRAN_TYPE=1099-OID&amp;pageType=4" xr:uid="{5854D5B2-E85F-427E-86FC-CDF7B1A06F74}"/>
-    <hyperlink ref="B54" r:id="rId5" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoForeignCurrGainLoss?ACCOUNT=X82865374&amp;SELECTED_YEAR_IND=0&amp;FCGL=Y" xr:uid="{15DDAA71-05A2-4BF1-986D-155DA4462084}"/>
-    <hyperlink ref="B56" r:id="rId6" tooltip="Details for Nondividend Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=X82865374&amp;TRS_TRAN_TYPE=1099-DIV&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=1&amp;txs=B" xr:uid="{C7AF1BF4-359E-4393-887E-27869A5042E1}"/>
-    <hyperlink ref="B57" r:id="rId7" tooltip="Details for Tax-Exempt Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=X82865374&amp;L2_TRAN_TYPE=1099-INT&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=0&amp;L2_INDEX=9&amp;txs=9&amp;BOX_N=8&amp;SORT_C=P" xr:uid="{9FADAA9F-7BA5-4927-9F01-BB01F049B381}"/>
-    <hyperlink ref="B61" r:id="rId8" tooltip="Details for Net Short-Term" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoRGL?ACCOUNT=X82865374&amp;SELECTED_YEAR=2024&amp;SELECTED_TERM=SHORT&amp;txs=F" xr:uid="{13810399-5AE3-4F61-8911-3E5A069270B9}"/>
-    <hyperlink ref="B62" r:id="rId9" tooltip="Details for Net Long-Term" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoRGL?ACCOUNT=X82865374&amp;SELECTED_YEAR=2024&amp;SELECTED_TERM=LONG&amp;txs=G" xr:uid="{29F566B1-7312-481E-96CB-D35A4BE33123}"/>
-    <hyperlink ref="B63" r:id="rId10" tooltip="Details for Reportable Bond Premium" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=X82865374&amp;SELECTED_YEAR_IND=0&amp;pageType=0" xr:uid="{759E95EE-49F9-4E8D-AE9A-1D9B505A6390}"/>
-    <hyperlink ref="B64" r:id="rId11" tooltip="Details for Realized Accrued Market Discount Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=X82865374&amp;SELECTED_YEAR_IND=0&amp;pageType=1" xr:uid="{A82AF2E5-CC22-4011-B9EC-6BDD973D779A}"/>
-    <hyperlink ref="B65" r:id="rId12" tooltip="Details for Ordinary Income or Loss" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=X82865374&amp;SELECTED_YEAR_IND=0&amp;pageType=2" xr:uid="{01C6184D-BD54-42A1-8F78-62FE13C0EA24}"/>
-    <hyperlink ref="B66" r:id="rId13" tooltip="Details for Reportable Acquisition Premium" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=X82865374&amp;SELECTED_YEAR_IND=0&amp;pageType=3" xr:uid="{F880BD40-9E81-4A20-AE56-95E87C08786E}"/>
-    <hyperlink ref="B76" r:id="rId14" tooltip="Details for Ordinary Dividends and Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80817344&amp;TRS_TRAN_TYPE=1099-DIV&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=1&amp;txs=B" xr:uid="{0DA854B3-9B63-4479-B2B2-C84A8C73374C}"/>
-    <hyperlink ref="B79" r:id="rId15" tooltip="Details for Interest Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80817344&amp;TRS_TRAN_TYPE=1099-INT&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=2&amp;txs=C" xr:uid="{69ED6A9E-18FC-4885-AA77-CDEB8DA4B253}"/>
-    <hyperlink ref="B80" r:id="rId16" tooltip="Details for Miscellaneous Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80817344&amp;TRS_TRAN_TYPE=1099-MISC&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=3&amp;txs=D" xr:uid="{2804DB18-0B72-43C2-9C7E-7B3C34932645}"/>
-    <hyperlink ref="B81" r:id="rId17" tooltip="Details for Original Issue Discount" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80817344&amp;SELECTED_YEAR_IND=0&amp;TRS_TRAN_TYPE=1099-OID&amp;pageType=4" xr:uid="{95391B1D-547F-4EC8-BDBA-EA3034A9BC4B}"/>
-    <hyperlink ref="B83" r:id="rId18" tooltip="Details for Nondividend Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80817344&amp;TRS_TRAN_TYPE=1099-DIV&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=1&amp;txs=B" xr:uid="{8BB23E09-E493-4388-A1D1-45806B856BD1}"/>
-    <hyperlink ref="B84" r:id="rId19" tooltip="Details for Tax-Exempt Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80817344&amp;L2_TRAN_TYPE=1099-INT&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=0&amp;L2_INDEX=9&amp;txs=9&amp;BOX_N=8&amp;SORT_C=P" xr:uid="{4A3CB314-292C-45EB-93AA-4DAFA721C823}"/>
-    <hyperlink ref="B88" r:id="rId20" tooltip="Details for Net Short-Term" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoRGL?ACCOUNT=Y80817344&amp;SELECTED_YEAR=2024&amp;SELECTED_TERM=SHORT&amp;txs=F" xr:uid="{CC0BE752-8F22-447F-8354-E3EBBC5E3FA6}"/>
-    <hyperlink ref="B89" r:id="rId21" tooltip="Details for Net Long-Term" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoRGL?ACCOUNT=Y80817344&amp;SELECTED_YEAR=2024&amp;SELECTED_TERM=LONG&amp;txs=G" xr:uid="{BED3D60B-926A-426C-BD5D-D3D8B35CE4C4}"/>
-    <hyperlink ref="B90" r:id="rId22" tooltip="Details for Reportable Bond Premium" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80817344&amp;SELECTED_YEAR_IND=0&amp;pageType=0" xr:uid="{7F9AEC1E-EF1B-4EC6-9D9D-CF3A62E06075}"/>
-    <hyperlink ref="B91" r:id="rId23" tooltip="Details for Realized Accrued Market Discount Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80817344&amp;SELECTED_YEAR_IND=0&amp;pageType=1" xr:uid="{EE0BF936-5584-475D-A1AA-164F94B264A9}"/>
-    <hyperlink ref="B92" r:id="rId24" tooltip="Details for Ordinary Income or Loss" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80817344&amp;SELECTED_YEAR_IND=0&amp;pageType=2" xr:uid="{841B448A-3C03-4DFC-9D8C-7D892E4A0A97}"/>
-    <hyperlink ref="B93" r:id="rId25" tooltip="Details for Reportable Acquisition Premium" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80817344&amp;SELECTED_YEAR_IND=0&amp;pageType=3" xr:uid="{F8BC197D-7CEA-4880-B281-06B4540E3B65}"/>
-    <hyperlink ref="B103" r:id="rId26" tooltip="Details for Ordinary Dividends and Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80570158&amp;TRS_TRAN_TYPE=1099-DIV&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=1&amp;txs=B" xr:uid="{0DB109E2-371E-443C-8BAC-4682AA2E0F79}"/>
-    <hyperlink ref="B106" r:id="rId27" tooltip="Details for Interest Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80570158&amp;TRS_TRAN_TYPE=1099-INT&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=2&amp;txs=C" xr:uid="{CF9C294B-9FD2-4B63-BB3F-41A532909618}"/>
-    <hyperlink ref="B107" r:id="rId28" tooltip="Details for Miscellaneous Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80570158&amp;TRS_TRAN_TYPE=1099-MISC&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=3&amp;txs=D" xr:uid="{62BEE76E-98E5-4127-B552-403018E2B7EA}"/>
-    <hyperlink ref="B108" r:id="rId29" tooltip="Details for Original Issue Discount" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80570158&amp;SELECTED_YEAR_IND=0&amp;TRS_TRAN_TYPE=1099-OID&amp;pageType=4" xr:uid="{30E6A617-5E69-4A9E-B624-6406B91B0C13}"/>
-    <hyperlink ref="B110" r:id="rId30" tooltip="Details for Nondividend Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80570158&amp;TRS_TRAN_TYPE=1099-DIV&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=1&amp;txs=B" xr:uid="{5679FA83-6181-41BA-8625-5DA302D35D9A}"/>
-    <hyperlink ref="B111" r:id="rId31" tooltip="Details for Tax-Exempt Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80570158&amp;L2_TRAN_TYPE=1099-INT&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=0&amp;L2_INDEX=9&amp;txs=9&amp;BOX_N=8&amp;SORT_C=P" xr:uid="{9CB0D3DD-C1C9-4ADB-BD4C-0E166CBC7BFA}"/>
-    <hyperlink ref="B115" r:id="rId32" tooltip="Details for Net Short-Term" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoRGL?ACCOUNT=Y80570158&amp;SELECTED_YEAR=2024&amp;SELECTED_TERM=SHORT&amp;txs=F" xr:uid="{8BAECF83-8613-44AD-AF6D-DC55F92C7B11}"/>
-    <hyperlink ref="B116" r:id="rId33" tooltip="Details for Net Long-Term" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoRGL?ACCOUNT=Y80570158&amp;SELECTED_YEAR=2024&amp;SELECTED_TERM=LONG&amp;txs=G" xr:uid="{99A6E161-3391-4135-929C-89DAC6A433D1}"/>
-    <hyperlink ref="B117" r:id="rId34" tooltip="Details for Reportable Bond Premium" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80570158&amp;SELECTED_YEAR_IND=0&amp;pageType=0" xr:uid="{B93F1FD8-E6F8-481F-9631-42279C53E67C}"/>
-    <hyperlink ref="B118" r:id="rId35" tooltip="Details for Realized Accrued Market Discount Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80570158&amp;SELECTED_YEAR_IND=0&amp;pageType=1" xr:uid="{2FC3E058-865D-4CC3-95AA-9221C943B67D}"/>
-    <hyperlink ref="B119" r:id="rId36" tooltip="Details for Ordinary Income or Loss" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80570158&amp;SELECTED_YEAR_IND=0&amp;pageType=2" xr:uid="{3FFF1721-3540-4716-9089-C450A20C6C0A}"/>
-    <hyperlink ref="B120" r:id="rId37" tooltip="Details for Reportable Acquisition Premium" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80570158&amp;SELECTED_YEAR_IND=0&amp;pageType=3" xr:uid="{CFBB5C71-EFC4-4759-83D4-AECC43A24260}"/>
-    <hyperlink ref="B130" r:id="rId38" tooltip="Details for Ordinary Dividends" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=X82865374&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=A&amp;BOX_N=1A&amp;L2_INDEX=1&amp;txs=1" xr:uid="{816E74BB-52DE-45A7-A987-126D37562630}"/>
-    <hyperlink ref="B135" r:id="rId39" tooltip="Details for Capital Gain Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=X82865374&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=F&amp;BOX_N=2&amp;L2_INDEX=2&amp;txs=2" xr:uid="{833EC093-47F0-4293-B452-464724672034}"/>
-    <hyperlink ref="B141" r:id="rId40" tooltip="Details for Nondividend Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=X82865374&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=L&amp;BOX_N=3&amp;L2_INDEX=3&amp;txs=3" xr:uid="{8D9797F1-3204-43AD-8E90-5806B6B41C85}"/>
-    <hyperlink ref="B142" r:id="rId41" tooltip="Details for Federal Income Tax Withheld" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=X82865374&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=M&amp;BOX_N=4&amp;L2_INDEX=4&amp;txs=4" xr:uid="{7CE2251A-9174-4D35-AE38-A904E2B26138}"/>
-    <hyperlink ref="B144" r:id="rId42" tooltip="Details for Foreign Tax Paid" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=X82865374&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=P&amp;BOX_N=7&amp;L2_INDEX=5&amp;txs=5" xr:uid="{8F3EEB72-7626-4054-9489-E9E35256DE42}"/>
-    <hyperlink ref="B153" r:id="rId43" tooltip="Details for Ordinary Dividends" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80817344&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=A&amp;BOX_N=1A&amp;L2_INDEX=1&amp;txs=1" xr:uid="{62AB7FAA-9720-4807-B77C-3F1F9D30478A}"/>
-    <hyperlink ref="B158" r:id="rId44" tooltip="Details for Capital Gain Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80817344&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=F&amp;BOX_N=2&amp;L2_INDEX=2&amp;txs=2" xr:uid="{82BE3218-8100-4136-B1AE-4D74D2D59F01}"/>
-    <hyperlink ref="B164" r:id="rId45" tooltip="Details for Nondividend Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80817344&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=L&amp;BOX_N=3&amp;L2_INDEX=3&amp;txs=3" xr:uid="{EF28B0E3-1772-4834-8306-0E14BC98A26F}"/>
-    <hyperlink ref="B165" r:id="rId46" tooltip="Details for Federal Income Tax Withheld" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80817344&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=M&amp;BOX_N=4&amp;L2_INDEX=4&amp;txs=4" xr:uid="{314C3CE7-76D3-4C4C-AD01-8B1B9687FAA5}"/>
-    <hyperlink ref="B167" r:id="rId47" tooltip="Details for Foreign Tax Paid" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80817344&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=P&amp;BOX_N=7&amp;L2_INDEX=5&amp;txs=5" xr:uid="{D2CBACEE-6F3A-4DC3-AD07-42F80111CA14}"/>
-    <hyperlink ref="B176" r:id="rId48" tooltip="Details for Ordinary Dividends" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80570158&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=A&amp;BOX_N=1A&amp;L2_INDEX=1&amp;txs=1" xr:uid="{BED4F7FF-BEB0-49C3-8DE7-35A8F8A7EEC6}"/>
-    <hyperlink ref="B181" r:id="rId49" tooltip="Details for Capital Gain Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80570158&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=F&amp;BOX_N=2&amp;L2_INDEX=2&amp;txs=2" xr:uid="{A49860B3-E5C2-4376-A22D-0A5C70ED69BE}"/>
-    <hyperlink ref="B187" r:id="rId50" tooltip="Details for Nondividend Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80570158&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=L&amp;BOX_N=3&amp;L2_INDEX=3&amp;txs=3" xr:uid="{25FCAE72-040E-4F23-8BE3-E3FDDC0876D0}"/>
-    <hyperlink ref="B188" r:id="rId51" tooltip="Details for Federal Income Tax Withheld" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80570158&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=M&amp;BOX_N=4&amp;L2_INDEX=4&amp;txs=4" xr:uid="{556503F8-053C-4DCA-AC00-EB8D0C2C068E}"/>
-    <hyperlink ref="B190" r:id="rId52" tooltip="Details for Foreign Tax Paid" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80570158&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=P&amp;BOX_N=7&amp;L2_INDEX=5&amp;txs=5" xr:uid="{B0E0CC07-D9BC-481E-95E6-A28F9AFEA5E3}"/>
+    <hyperlink ref="B47" r:id="rId1" tooltip="Details for Ordinary Dividends and Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=X82865374&amp;TRS_TRAN_TYPE=1099-DIV&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=1&amp;txs=B" xr:uid="{1CD51B58-6A11-4DC5-8A80-9CCAEEF0E29C}"/>
+    <hyperlink ref="B50" r:id="rId2" tooltip="Details for Interest Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=X82865374&amp;TRS_TRAN_TYPE=1099-INT&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=2&amp;txs=C" xr:uid="{1E164B20-4BC7-4A31-89A0-25B5A2BDD0DC}"/>
+    <hyperlink ref="B51" r:id="rId3" tooltip="Details for Miscellaneous Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=X82865374&amp;TRS_TRAN_TYPE=1099-MISC&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=3&amp;txs=D" xr:uid="{0E88321C-3E19-484D-AC02-F09F9943D234}"/>
+    <hyperlink ref="B52" r:id="rId4" tooltip="Details for Original Issue Discount" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=X82865374&amp;SELECTED_YEAR_IND=0&amp;TRS_TRAN_TYPE=1099-OID&amp;pageType=4" xr:uid="{5854D5B2-E85F-427E-86FC-CDF7B1A06F74}"/>
+    <hyperlink ref="B53" r:id="rId5" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoForeignCurrGainLoss?ACCOUNT=X82865374&amp;SELECTED_YEAR_IND=0&amp;FCGL=Y" xr:uid="{15DDAA71-05A2-4BF1-986D-155DA4462084}"/>
+    <hyperlink ref="B55" r:id="rId6" tooltip="Details for Nondividend Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=X82865374&amp;TRS_TRAN_TYPE=1099-DIV&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=1&amp;txs=B" xr:uid="{C7AF1BF4-359E-4393-887E-27869A5042E1}"/>
+    <hyperlink ref="B56" r:id="rId7" tooltip="Details for Tax-Exempt Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=X82865374&amp;L2_TRAN_TYPE=1099-INT&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=0&amp;L2_INDEX=9&amp;txs=9&amp;BOX_N=8&amp;SORT_C=P" xr:uid="{9FADAA9F-7BA5-4927-9F01-BB01F049B381}"/>
+    <hyperlink ref="B60" r:id="rId8" tooltip="Details for Net Short-Term" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoRGL?ACCOUNT=X82865374&amp;SELECTED_YEAR=2024&amp;SELECTED_TERM=SHORT&amp;txs=F" xr:uid="{13810399-5AE3-4F61-8911-3E5A069270B9}"/>
+    <hyperlink ref="B61" r:id="rId9" tooltip="Details for Net Long-Term" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoRGL?ACCOUNT=X82865374&amp;SELECTED_YEAR=2024&amp;SELECTED_TERM=LONG&amp;txs=G" xr:uid="{29F566B1-7312-481E-96CB-D35A4BE33123}"/>
+    <hyperlink ref="B62" r:id="rId10" tooltip="Details for Reportable Bond Premium" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=X82865374&amp;SELECTED_YEAR_IND=0&amp;pageType=0" xr:uid="{759E95EE-49F9-4E8D-AE9A-1D9B505A6390}"/>
+    <hyperlink ref="B63" r:id="rId11" tooltip="Details for Realized Accrued Market Discount Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=X82865374&amp;SELECTED_YEAR_IND=0&amp;pageType=1" xr:uid="{A82AF2E5-CC22-4011-B9EC-6BDD973D779A}"/>
+    <hyperlink ref="B64" r:id="rId12" tooltip="Details for Ordinary Income or Loss" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=X82865374&amp;SELECTED_YEAR_IND=0&amp;pageType=2" xr:uid="{01C6184D-BD54-42A1-8F78-62FE13C0EA24}"/>
+    <hyperlink ref="B65" r:id="rId13" tooltip="Details for Reportable Acquisition Premium" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=X82865374&amp;SELECTED_YEAR_IND=0&amp;pageType=3" xr:uid="{F880BD40-9E81-4A20-AE56-95E87C08786E}"/>
+    <hyperlink ref="B75" r:id="rId14" tooltip="Details for Ordinary Dividends and Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80817344&amp;TRS_TRAN_TYPE=1099-DIV&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=1&amp;txs=B" xr:uid="{0DA854B3-9B63-4479-B2B2-C84A8C73374C}"/>
+    <hyperlink ref="B78" r:id="rId15" tooltip="Details for Interest Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80817344&amp;TRS_TRAN_TYPE=1099-INT&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=2&amp;txs=C" xr:uid="{69ED6A9E-18FC-4885-AA77-CDEB8DA4B253}"/>
+    <hyperlink ref="B79" r:id="rId16" tooltip="Details for Miscellaneous Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80817344&amp;TRS_TRAN_TYPE=1099-MISC&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=3&amp;txs=D" xr:uid="{2804DB18-0B72-43C2-9C7E-7B3C34932645}"/>
+    <hyperlink ref="B80" r:id="rId17" tooltip="Details for Original Issue Discount" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80817344&amp;SELECTED_YEAR_IND=0&amp;TRS_TRAN_TYPE=1099-OID&amp;pageType=4" xr:uid="{95391B1D-547F-4EC8-BDBA-EA3034A9BC4B}"/>
+    <hyperlink ref="B82" r:id="rId18" tooltip="Details for Nondividend Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80817344&amp;TRS_TRAN_TYPE=1099-DIV&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=1&amp;txs=B" xr:uid="{8BB23E09-E493-4388-A1D1-45806B856BD1}"/>
+    <hyperlink ref="B83" r:id="rId19" tooltip="Details for Tax-Exempt Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80817344&amp;L2_TRAN_TYPE=1099-INT&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=0&amp;L2_INDEX=9&amp;txs=9&amp;BOX_N=8&amp;SORT_C=P" xr:uid="{4A3CB314-292C-45EB-93AA-4DAFA721C823}"/>
+    <hyperlink ref="B87" r:id="rId20" tooltip="Details for Net Short-Term" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoRGL?ACCOUNT=Y80817344&amp;SELECTED_YEAR=2024&amp;SELECTED_TERM=SHORT&amp;txs=F" xr:uid="{CC0BE752-8F22-447F-8354-E3EBBC5E3FA6}"/>
+    <hyperlink ref="B88" r:id="rId21" tooltip="Details for Net Long-Term" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoRGL?ACCOUNT=Y80817344&amp;SELECTED_YEAR=2024&amp;SELECTED_TERM=LONG&amp;txs=G" xr:uid="{BED3D60B-926A-426C-BD5D-D3D8B35CE4C4}"/>
+    <hyperlink ref="B89" r:id="rId22" tooltip="Details for Reportable Bond Premium" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80817344&amp;SELECTED_YEAR_IND=0&amp;pageType=0" xr:uid="{7F9AEC1E-EF1B-4EC6-9D9D-CF3A62E06075}"/>
+    <hyperlink ref="B90" r:id="rId23" tooltip="Details for Realized Accrued Market Discount Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80817344&amp;SELECTED_YEAR_IND=0&amp;pageType=1" xr:uid="{EE0BF936-5584-475D-A1AA-164F94B264A9}"/>
+    <hyperlink ref="B91" r:id="rId24" tooltip="Details for Ordinary Income or Loss" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80817344&amp;SELECTED_YEAR_IND=0&amp;pageType=2" xr:uid="{841B448A-3C03-4DFC-9D8C-7D892E4A0A97}"/>
+    <hyperlink ref="B92" r:id="rId25" tooltip="Details for Reportable Acquisition Premium" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80817344&amp;SELECTED_YEAR_IND=0&amp;pageType=3" xr:uid="{F8BC197D-7CEA-4880-B281-06B4540E3B65}"/>
+    <hyperlink ref="B102" r:id="rId26" tooltip="Details for Ordinary Dividends and Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80570158&amp;TRS_TRAN_TYPE=1099-DIV&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=1&amp;txs=B" xr:uid="{0DB109E2-371E-443C-8BAC-4682AA2E0F79}"/>
+    <hyperlink ref="B105" r:id="rId27" tooltip="Details for Interest Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80570158&amp;TRS_TRAN_TYPE=1099-INT&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=2&amp;txs=C" xr:uid="{CF9C294B-9FD2-4B63-BB3F-41A532909618}"/>
+    <hyperlink ref="B106" r:id="rId28" tooltip="Details for Miscellaneous Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80570158&amp;TRS_TRAN_TYPE=1099-MISC&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=3&amp;txs=D" xr:uid="{62BEE76E-98E5-4127-B552-403018E2B7EA}"/>
+    <hyperlink ref="B107" r:id="rId29" tooltip="Details for Original Issue Discount" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80570158&amp;SELECTED_YEAR_IND=0&amp;TRS_TRAN_TYPE=1099-OID&amp;pageType=4" xr:uid="{30E6A617-5E69-4A9E-B624-6406B91B0C13}"/>
+    <hyperlink ref="B109" r:id="rId30" tooltip="Details for Nondividend Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL1T1?ACCOUNT=Y80570158&amp;TRS_TRAN_TYPE=1099-DIV&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=1&amp;txs=B" xr:uid="{5679FA83-6181-41BA-8625-5DA302D35D9A}"/>
+    <hyperlink ref="B110" r:id="rId31" tooltip="Details for Tax-Exempt Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80570158&amp;L2_TRAN_TYPE=1099-INT&amp;SELECTED_YEAR_IND=0&amp;L1T1_INDEX=0&amp;L2_INDEX=9&amp;txs=9&amp;BOX_N=8&amp;SORT_C=P" xr:uid="{9CB0D3DD-C1C9-4ADB-BD4C-0E166CBC7BFA}"/>
+    <hyperlink ref="B114" r:id="rId32" tooltip="Details for Net Short-Term" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoRGL?ACCOUNT=Y80570158&amp;SELECTED_YEAR=2024&amp;SELECTED_TERM=SHORT&amp;txs=F" xr:uid="{8BAECF83-8613-44AD-AF6D-DC55F92C7B11}"/>
+    <hyperlink ref="B115" r:id="rId33" tooltip="Details for Net Long-Term" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoRGL?ACCOUNT=Y80570158&amp;SELECTED_YEAR=2024&amp;SELECTED_TERM=LONG&amp;txs=G" xr:uid="{99A6E161-3391-4135-929C-89DAC6A433D1}"/>
+    <hyperlink ref="B116" r:id="rId34" tooltip="Details for Reportable Bond Premium" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80570158&amp;SELECTED_YEAR_IND=0&amp;pageType=0" xr:uid="{B93F1FD8-E6F8-481F-9631-42279C53E67C}"/>
+    <hyperlink ref="B117" r:id="rId35" tooltip="Details for Realized Accrued Market Discount Income" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80570158&amp;SELECTED_YEAR_IND=0&amp;pageType=1" xr:uid="{2FC3E058-865D-4CC3-95AA-9221C943B67D}"/>
+    <hyperlink ref="B118" r:id="rId36" tooltip="Details for Ordinary Income or Loss" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80570158&amp;SELECTED_YEAR_IND=0&amp;pageType=2" xr:uid="{3FFF1721-3540-4716-9089-C450A20C6C0A}"/>
+    <hyperlink ref="B119" r:id="rId37" tooltip="Details for Reportable Acquisition Premium" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoDetails?ACCOUNT=Y80570158&amp;SELECTED_YEAR_IND=0&amp;pageType=3" xr:uid="{CFBB5C71-EFC4-4759-83D4-AECC43A24260}"/>
+    <hyperlink ref="B129" r:id="rId38" tooltip="Details for Ordinary Dividends" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=X82865374&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=A&amp;BOX_N=1A&amp;L2_INDEX=1&amp;txs=1" xr:uid="{816E74BB-52DE-45A7-A987-126D37562630}"/>
+    <hyperlink ref="B134" r:id="rId39" tooltip="Details for Capital Gain Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=X82865374&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=F&amp;BOX_N=2&amp;L2_INDEX=2&amp;txs=2" xr:uid="{833EC093-47F0-4293-B452-464724672034}"/>
+    <hyperlink ref="B140" r:id="rId40" tooltip="Details for Nondividend Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=X82865374&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=L&amp;BOX_N=3&amp;L2_INDEX=3&amp;txs=3" xr:uid="{8D9797F1-3204-43AD-8E90-5806B6B41C85}"/>
+    <hyperlink ref="B141" r:id="rId41" tooltip="Details for Federal Income Tax Withheld" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=X82865374&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=M&amp;BOX_N=4&amp;L2_INDEX=4&amp;txs=4" xr:uid="{7CE2251A-9174-4D35-AE38-A904E2B26138}"/>
+    <hyperlink ref="B143" r:id="rId42" tooltip="Details for Foreign Tax Paid" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=X82865374&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=P&amp;BOX_N=7&amp;L2_INDEX=5&amp;txs=5" xr:uid="{8F3EEB72-7626-4054-9489-E9E35256DE42}"/>
+    <hyperlink ref="B152" r:id="rId43" tooltip="Details for Ordinary Dividends" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80817344&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=A&amp;BOX_N=1A&amp;L2_INDEX=1&amp;txs=1" xr:uid="{62AB7FAA-9720-4807-B77C-3F1F9D30478A}"/>
+    <hyperlink ref="B157" r:id="rId44" tooltip="Details for Capital Gain Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80817344&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=F&amp;BOX_N=2&amp;L2_INDEX=2&amp;txs=2" xr:uid="{82BE3218-8100-4136-B1AE-4D74D2D59F01}"/>
+    <hyperlink ref="B163" r:id="rId45" tooltip="Details for Nondividend Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80817344&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=L&amp;BOX_N=3&amp;L2_INDEX=3&amp;txs=3" xr:uid="{EF28B0E3-1772-4834-8306-0E14BC98A26F}"/>
+    <hyperlink ref="B164" r:id="rId46" tooltip="Details for Federal Income Tax Withheld" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80817344&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=M&amp;BOX_N=4&amp;L2_INDEX=4&amp;txs=4" xr:uid="{314C3CE7-76D3-4C4C-AD01-8B1B9687FAA5}"/>
+    <hyperlink ref="B166" r:id="rId47" tooltip="Details for Foreign Tax Paid" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80817344&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=P&amp;BOX_N=7&amp;L2_INDEX=5&amp;txs=5" xr:uid="{D2CBACEE-6F3A-4DC3-AD07-42F80111CA14}"/>
+    <hyperlink ref="B175" r:id="rId48" tooltip="Details for Ordinary Dividends" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80570158&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=A&amp;BOX_N=1A&amp;L2_INDEX=1&amp;txs=1" xr:uid="{BED4F7FF-BEB0-49C3-8DE7-35A8F8A7EEC6}"/>
+    <hyperlink ref="B180" r:id="rId49" tooltip="Details for Capital Gain Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80570158&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=F&amp;BOX_N=2&amp;L2_INDEX=2&amp;txs=2" xr:uid="{A49860B3-E5C2-4376-A22D-0A5C70ED69BE}"/>
+    <hyperlink ref="B186" r:id="rId50" tooltip="Details for Nondividend Distributions" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80570158&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=L&amp;BOX_N=3&amp;L2_INDEX=3&amp;txs=3" xr:uid="{25FCAE72-040E-4F23-8BE3-E3FDDC0876D0}"/>
+    <hyperlink ref="B187" r:id="rId51" tooltip="Details for Federal Income Tax Withheld" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80570158&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=M&amp;BOX_N=4&amp;L2_INDEX=4&amp;txs=4" xr:uid="{556503F8-053C-4DCA-AC00-EB8D0C2C068E}"/>
+    <hyperlink ref="B189" r:id="rId52" tooltip="Details for Foreign Tax Paid" display="https://oltx.fidelity.com/ftgw/fbc/ofaccounts/taxInfoL2?ACCOUNT=Y80570158&amp;L2_TRAN_TYPE=1099-DIV&amp;txn=1099-DIV&amp;L1T1_INDEX=1&amp;SELECTED_YEAR_IND=0&amp;SORT_C=P&amp;BOX_N=7&amp;L2_INDEX=5&amp;txs=5" xr:uid="{B0E0CC07-D9BC-481E-95E6-A28F9AFEA5E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId53"/>
@@ -4906,11 +4894,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A1" s="72" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="74"/>
+      <c r="A1" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="76"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="65">
@@ -5881,11 +5869,11 @@
       </c>
     </row>
     <row r="123" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A123" s="79" t="s">
-        <v>80</v>
-      </c>
-      <c r="B123" s="80"/>
-      <c r="C123" s="81"/>
+      <c r="A123" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="B123" s="72"/>
+      <c r="C123" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Still more refactoring and "cleanup."
</commit_message>
<xml_diff>
--- a/myStudies/RothConversion.xlsx
+++ b/myStudies/RothConversion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkrat\git\MyStudiesRepo\myStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C5171A-C33A-44D2-B5D9-7CD208832C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B45D21-8D92-4794-AF85-9A0C067E2C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" activeTab="2" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
   </bookViews>
@@ -267,9 +267,6 @@
     <t>Investments</t>
   </si>
   <si>
-    <t>Standard Deduction Current Year</t>
-  </si>
-  <si>
     <t>IRMAA Multipliers</t>
   </si>
   <si>
@@ -279,12 +276,6 @@
     <t>Social Security AGI Tax Rates</t>
   </si>
   <si>
-    <t>Current Date</t>
-  </si>
-  <si>
-    <t>Part B Premium Current Year</t>
-  </si>
-  <si>
     <t>Expected Life Lengths</t>
   </si>
   <si>
@@ -300,18 +291,12 @@
     <t>Basis</t>
   </si>
   <si>
-    <t>SSA</t>
-  </si>
-  <si>
     <t>Short-Term</t>
   </si>
   <si>
     <t>Long-Term</t>
   </si>
   <si>
-    <t>Max Capital Gains Loss</t>
-  </si>
-  <si>
     <t>Miscellaneous Data</t>
   </si>
   <si>
@@ -324,9 +309,6 @@
     <t>Diem-Tran-TSP</t>
   </si>
   <si>
-    <t>Medicare Tax Threshold</t>
-  </si>
-  <si>
     <t>Additional Medicare Tax</t>
   </si>
   <si>
@@ -336,15 +318,6 @@
     <t>Age of RMD</t>
   </si>
   <si>
-    <t>Divisor Current Year</t>
-  </si>
-  <si>
-    <t>Balance Beginning of Current Year</t>
-  </si>
-  <si>
-    <t>Current Balance</t>
-  </si>
-  <si>
     <t>Account Owners</t>
   </si>
   <si>
@@ -385,6 +358,33 @@
   </si>
   <si>
     <t>IRA - BDA (238262976)</t>
+  </si>
+  <si>
+    <t>Standard Deduction Base Year</t>
+  </si>
+  <si>
+    <t>Divisor Base Year</t>
+  </si>
+  <si>
+    <t>Balance Beginning of Base Year</t>
+  </si>
+  <si>
+    <t>Base Balance</t>
+  </si>
+  <si>
+    <t>Max Capital Gains Loss Base Year</t>
+  </si>
+  <si>
+    <t>Medicare Tax Threshold Base Year</t>
+  </si>
+  <si>
+    <t>Social Security Income</t>
+  </si>
+  <si>
+    <t>Part B Standard Premium Base Year</t>
+  </si>
+  <si>
+    <t>Base Date</t>
   </si>
 </sst>
 </file>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="71"/>
       <c r="C17" s="72"/>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" s="71"/>
       <c r="C21" s="72"/>
@@ -2096,7 +2096,7 @@
     </row>
     <row r="25" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="70" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25" s="71"/>
       <c r="C25" s="72"/>
@@ -2219,7 +2219,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="71"/>
       <c r="C1" s="72"/>
@@ -2631,8 +2631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8746EC-93A7-4CC1-BFC6-CA309B41AD35}">
   <dimension ref="A1:I268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2654,7 +2654,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B1" s="71"/>
       <c r="C1" s="72"/>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="B2" s="33">
         <v>45422</v>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="B4" s="15">
         <v>29200</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="B5" s="26">
         <v>174.7</v>
@@ -2716,7 +2716,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="B6" s="15">
         <v>3000</v>
@@ -2731,10 +2731,10 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="36">
-        <v>0.05</v>
+        <v>107</v>
+      </c>
+      <c r="B7" s="37">
+        <v>250000</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>41</v>
@@ -2746,36 +2746,36 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="36">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>87</v>
+      <c r="A9" s="14" t="s">
+        <v>70</v>
       </c>
       <c r="B9" s="36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="36">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="37">
-        <v>250000</v>
-      </c>
+      <c r="C10" s="6"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B11" s="36">
         <v>8.9999999999999993E-3</v>
@@ -2784,7 +2784,7 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B12" s="36">
         <v>3.7999999999999999E-2</v>
@@ -2793,7 +2793,7 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="73" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B13" s="71"/>
       <c r="C13" s="72"/>
@@ -2823,7 +2823,7 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="73" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B16" s="71"/>
       <c r="C16" s="72"/>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>62</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>62</v>
@@ -2856,7 +2856,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>63</v>
@@ -2865,28 +2865,28 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B20" s="40"/>
       <c r="C20" s="41"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B21" s="40"/>
       <c r="C21" s="41"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="41"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="73" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B23" s="71"/>
       <c r="C23" s="72"/>
@@ -2896,7 +2896,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B24" s="2">
         <v>73</v>
@@ -2908,7 +2908,7 @@
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B25" s="2">
         <v>73</v>
@@ -2918,7 +2918,7 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="73" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B26" s="71"/>
       <c r="C26" s="72"/>
@@ -2928,7 +2928,7 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B27" s="2">
         <v>17.2</v>
@@ -2937,7 +2937,7 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="73" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B28" s="71"/>
       <c r="C28" s="72"/>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B29" s="15">
         <v>41925.5</v>
@@ -2956,7 +2956,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B30" s="15">
         <v>2082478.98</v>
@@ -2968,7 +2968,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B31" s="15">
         <v>1049867.8400000001</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B32" s="15">
         <v>400000</v>
@@ -2992,7 +2992,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B33" s="15">
         <v>130000</v>
@@ -3001,7 +3001,7 @@
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B34" s="15">
         <v>170000</v>
@@ -3013,7 +3013,7 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" s="73" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B35" s="71"/>
       <c r="C35" s="72"/>
@@ -3023,7 +3023,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B36" s="15">
         <v>41925</v>
@@ -3035,7 +3035,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B37" s="15">
         <v>2200000</v>
@@ -3047,7 +3047,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B38" s="15">
         <v>1009000</v>
@@ -3059,7 +3059,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B39" s="15">
         <v>400000</v>
@@ -3071,7 +3071,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B40" s="15">
         <v>200000</v>
@@ -3083,7 +3083,7 @@
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B41" s="15">
         <v>300000</v>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="42" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42" s="73" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B42" s="71"/>
       <c r="C42" s="72"/>
@@ -3105,7 +3105,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B43" s="15">
         <v>250000</v>
@@ -3117,7 +3117,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B44" s="15">
         <v>130000</v>
@@ -3129,7 +3129,7 @@
     </row>
     <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B45" s="15">
         <v>130000</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="46" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A46" s="73" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B46" s="71"/>
       <c r="C46" s="72"/>
@@ -3174,14 +3174,14 @@
     </row>
     <row r="49" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="77" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B49" s="78"/>
       <c r="C49" s="79"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B50" s="21">
         <v>-10950</v>
@@ -3190,7 +3190,7 @@
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B51" s="16">
         <v>-17755</v>
@@ -3221,7 +3221,7 @@
     </row>
     <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B54" s="34" t="s">
         <v>62</v>
@@ -3233,7 +3233,7 @@
     </row>
     <row r="55" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A55" s="73" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B55" s="71"/>
       <c r="C55" s="72"/>
@@ -3256,7 +3256,7 @@
     </row>
     <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B57" s="15">
         <f>71065.98-50692.01</f>
@@ -3266,7 +3266,7 @@
     </row>
     <row r="58" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A58" s="73" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B58" s="71"/>
       <c r="C58" s="72"/>
@@ -3274,7 +3274,7 @@
     </row>
     <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B59" s="35">
         <v>2025</v>
@@ -3360,7 +3360,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B1" s="71"/>
       <c r="C1" s="72"/>
@@ -3448,7 +3448,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="43" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B11" s="44">
         <v>0</v>
@@ -3505,7 +3505,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -3524,7 +3524,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="57" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B18"/>
     </row>
@@ -3533,7 +3533,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3541,15 +3541,15 @@
         <v>12</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="45" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3557,7 +3557,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="55" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3741,7 +3741,7 @@
     </row>
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="59" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B44" s="49">
         <v>0</v>
@@ -3749,7 +3749,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="50" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B45" s="51">
         <v>0</v>
@@ -3757,7 +3757,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="80" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B47" s="80"/>
       <c r="C47" s="80"/>
@@ -3830,7 +3830,7 @@
     </row>
     <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="43" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B57" s="44">
         <v>0</v>
@@ -3882,7 +3882,7 @@
     </row>
     <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="60" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B64"/>
     </row>
@@ -3891,7 +3891,7 @@
         <v>11</v>
       </c>
       <c r="B65" s="46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3899,15 +3899,15 @@
         <v>12</v>
       </c>
       <c r="B66" s="46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="45" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B67" s="46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -3915,7 +3915,7 @@
         <v>13</v>
       </c>
       <c r="B68" s="55" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.25">
@@ -4057,7 +4057,7 @@
         <v>37</v>
       </c>
       <c r="B86" s="46" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4078,7 +4078,7 @@
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="59" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B89" s="49">
         <v>0</v>
@@ -4086,7 +4086,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="50" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B90" s="51">
         <v>0</v>
@@ -4094,7 +4094,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="80" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B92" s="80"/>
       <c r="C92" s="80"/>
@@ -4167,7 +4167,7 @@
     </row>
     <row r="102" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="43" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B102" s="44">
         <v>29.18</v>
@@ -4219,7 +4219,7 @@
     </row>
     <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="60" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B109"/>
     </row>
@@ -4228,7 +4228,7 @@
         <v>11</v>
       </c>
       <c r="B110" s="46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4236,15 +4236,15 @@
         <v>12</v>
       </c>
       <c r="B111" s="46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="45" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B112" s="46" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -4252,7 +4252,7 @@
         <v>13</v>
       </c>
       <c r="B113" s="55" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="18" x14ac:dyDescent="0.25">
@@ -4394,7 +4394,7 @@
         <v>37</v>
       </c>
       <c r="B132" s="46" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4415,7 +4415,7 @@
     </row>
     <row r="135" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="59" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B135" s="49">
         <v>0</v>
@@ -4423,7 +4423,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="52" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B136" s="42"/>
     </row>

</xml_diff>

<commit_message>
Good cleanup and removed a couple of latent bugs.
</commit_message>
<xml_diff>
--- a/myStudies/RothConversion.xlsx
+++ b/myStudies/RothConversion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkrat\git\MyStudiesRepo\myStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B45D21-8D92-4794-AF85-9A0C067E2C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98F36E1-2137-48F9-8143-75430EC9EC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="735" activeTab="2" xr2:uid="{61290AE9-9247-4055-A5C3-1005466886B7}"/>
   </bookViews>
@@ -363,9 +363,6 @@
     <t>Standard Deduction Base Year</t>
   </si>
   <si>
-    <t>Divisor Base Year</t>
-  </si>
-  <si>
     <t>Balance Beginning of Base Year</t>
   </si>
   <si>
@@ -385,6 +382,9 @@
   </si>
   <si>
     <t>Base Date</t>
+  </si>
+  <si>
+    <t>Inherited IRA Divisor for Base Year</t>
   </si>
 </sst>
 </file>
@@ -2631,8 +2631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8746EC-93A7-4CC1-BFC6-CA309B41AD35}">
   <dimension ref="A1:I268"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="33">
         <v>45422</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B5" s="26">
         <v>174.7</v>
@@ -2716,7 +2716,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="15">
         <v>3000</v>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="37">
         <v>250000</v>
@@ -2918,7 +2918,7 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="73" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B26" s="71"/>
       <c r="C26" s="72"/>
@@ -2937,7 +2937,7 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="73" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B28" s="71"/>
       <c r="C28" s="72"/>
@@ -3013,7 +3013,7 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" s="73" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35" s="71"/>
       <c r="C35" s="72"/>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="46" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A46" s="73" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B46" s="71"/>
       <c r="C46" s="72"/>

</xml_diff>